<commit_message>
Kayser standard deviations corrected via t-test
</commit_message>
<xml_diff>
--- a/experimental_data/liver_volume/Kayser1987.xlsx
+++ b/experimental_data/liver_volume/Kayser1987.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="145" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="136" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Ducry1979" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="34">
   <si>
     <t>Kayser1987 – Height and weight in human beings</t>
   </si>
@@ -38,7 +38,19 @@
     <t>subjects</t>
   </si>
   <si>
+    <t>large sample</t>
+  </si>
+  <si>
+    <t>small sample</t>
+  </si>
+  <si>
     <t>Table 21 – 22</t>
+  </si>
+  <si>
+    <t>Size (n&gt;60)</t>
+  </si>
+  <si>
+    <t>size (t-distribution) </t>
   </si>
   <si>
     <t>study</t>
@@ -89,6 +101,9 @@
     <t>livWeight95</t>
   </si>
   <si>
+    <t>livWeightSdBase</t>
+  </si>
+  <si>
     <t>livWeightSd</t>
   </si>
   <si>
@@ -113,7 +128,7 @@
     <numFmt formatCode="0.00" numFmtId="165"/>
     <numFmt formatCode="0.0" numFmtId="166"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -143,11 +158,28 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF3333FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -219,7 +251,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -260,11 +292,19 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -281,7 +321,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -331,9 +371,9 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3333FF"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -375,7 +415,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -605,116 +645,6 @@
               </c:numRef>
             </c:minus>
           </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ducry1979!$H$45:$H$78</c:f>
-              <c:strCache>
-                <c:ptCount val="34"/>
-                <c:pt idx="0">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>118.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>155.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>183.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>413.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>505.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>527.4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>553.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>618.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>612</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>752.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>911.8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>845.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1095</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>989.1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1050.2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1194.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1307.6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1347.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1398.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1504.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1456.3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1543.3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1591.6</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1557.9</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1495.2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1408.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1252.3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1172.7</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1035</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
               <c:f>Ducry1979!$E$11:$E$44</c:f>
@@ -964,7 +894,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -978,82 +908,82 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="34"/>
                   <c:pt idx="0">
-                    <c:v>1.93877551020408</c:v>
+                    <c:v>46.0025305788548</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.14285714285714</c:v>
+                    <c:v>58.4668055133746</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.22448979591836</c:v>
+                    <c:v>46.1620518074322</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.84693877551021</c:v>
+                    <c:v>68.221593032815</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>19.4387755102041</c:v>
+                    <c:v>128.942249502593</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>16.1734693877551</c:v>
+                    <c:v>97.0408163265306</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>16.5816326530612</c:v>
+                    <c:v>96.6867023379961</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>15.5612244897959</c:v>
+                    <c:v>100.848260868082</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>56.1224489795919</c:v>
+                    <c:v>296.972085935822</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>28.5204081632653</c:v>
+                    <c:v>178.109891893097</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>27.0918367346939</c:v>
+                    <c:v>150.840963095038</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>39.9489795918368</c:v>
+                    <c:v>174.133564938385</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>31.4795918367347</c:v>
+                    <c:v>196.589988010807</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>39.4897959183673</c:v>
+                    <c:v>176.603736182126</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>41.6326530612245</c:v>
+                    <c:v>212.285710361822</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>58.6734693877551</c:v>
+                    <c:v>275.202965499844</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>61.9897959183674</c:v>
+                    <c:v>240.085447226633</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>48.7755102040816</c:v>
+                    <c:v>154.241706281682</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>98.265306122449</c:v>
+                    <c:v>340.401005650781</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>69.8469387755101</c:v>
+                    <c:v>304.455747638121</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>57.6530612244898</c:v>
+                    <c:v>191.213572097021</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>56.4285714285715</c:v>
+                    <c:v>298.59193367729</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>108.724489795918</c:v>
+                    <c:v>434.897959183673</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>75.4591836734693</c:v>
+                    <c:v>452.755102040816</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>78.469387755102</c:v>
+                    <c:v>400.116939382944</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>54.1326530612246</c:v>
+                    <c:v>324.795918367347</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>358.176347223154</c:v>
@@ -1089,82 +1019,82 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="34"/>
                   <c:pt idx="0">
-                    <c:v>1.93877551020408</c:v>
+                    <c:v>46.0025305788548</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.14285714285714</c:v>
+                    <c:v>58.4668055133746</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.22448979591836</c:v>
+                    <c:v>46.1620518074322</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.84693877551021</c:v>
+                    <c:v>68.221593032815</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>19.4387755102041</c:v>
+                    <c:v>128.942249502593</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>16.1734693877551</c:v>
+                    <c:v>97.0408163265306</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>16.5816326530612</c:v>
+                    <c:v>96.6867023379961</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>15.5612244897959</c:v>
+                    <c:v>100.848260868082</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>56.1224489795919</c:v>
+                    <c:v>296.972085935822</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>28.5204081632653</c:v>
+                    <c:v>178.109891893097</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>27.0918367346939</c:v>
+                    <c:v>150.840963095038</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>39.9489795918368</c:v>
+                    <c:v>174.133564938385</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>31.4795918367347</c:v>
+                    <c:v>196.589988010807</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>39.4897959183673</c:v>
+                    <c:v>176.603736182126</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>41.6326530612245</c:v>
+                    <c:v>212.285710361822</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>58.6734693877551</c:v>
+                    <c:v>275.202965499844</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>61.9897959183674</c:v>
+                    <c:v>240.085447226633</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>48.7755102040816</c:v>
+                    <c:v>154.241706281682</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>98.265306122449</c:v>
+                    <c:v>340.401005650781</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>69.8469387755101</c:v>
+                    <c:v>304.455747638121</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>57.6530612244898</c:v>
+                    <c:v>191.213572097021</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>56.4285714285715</c:v>
+                    <c:v>298.59193367729</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>108.724489795918</c:v>
+                    <c:v>434.897959183673</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>75.4591836734693</c:v>
+                    <c:v>452.755102040816</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>78.469387755102</c:v>
+                    <c:v>400.116939382944</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>54.1326530612246</c:v>
+                    <c:v>324.795918367347</c:v>
                   </c:pt>
                   <c:pt idx="26">
                     <c:v>358.176347223154</c:v>
@@ -1194,116 +1124,6 @@
               </c:numRef>
             </c:minus>
           </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ducry1979!$H$45:$H$78</c:f>
-              <c:strCache>
-                <c:ptCount val="34"/>
-                <c:pt idx="0">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>118.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>155.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>183.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>413.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>505.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>527.4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>553.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>618.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>612</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>752.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>911.8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>845.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1095</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>989.1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1050.2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1194.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1307.6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1347.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1398.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1504.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1456.3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1543.3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1591.6</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1557.9</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1495.2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1408.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1252.3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1172.7</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1035</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
               <c:f>Ducry1979!$E$45:$E$78</c:f>
@@ -1527,11 +1347,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="3866723"/>
-        <c:axId val="91901193"/>
+        <c:axId val="74802383"/>
+        <c:axId val="45850292"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3866723"/>
+        <c:axId val="74802383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1367,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age [years]</a:t>
                 </a:r>
               </a:p>
@@ -1565,11 +1385,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91901193"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="45850292"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91901193"/>
+        <c:axId val="45850292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500"/>
@@ -1586,7 +1406,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>liver weight [g]</a:t>
                 </a:r>
               </a:p>
@@ -1604,8 +1424,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3866723"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="74802383"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1643,16 +1463,16 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>413280</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>508320</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1667,8 +1487,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8316360" y="720720"/>
-          <a:ext cx="4653720" cy="4183560"/>
+          <a:off x="10037520" y="634320"/>
+          <a:ext cx="4653360" cy="4182840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1683,15 +1503,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>481680</xdr:colOff>
+      <xdr:colOff>508680</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>737280</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:colOff>763920</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1706,8 +1526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13038480" y="845640"/>
-          <a:ext cx="4319640" cy="4497840"/>
+          <a:off x="13065480" y="845640"/>
+          <a:ext cx="4319280" cy="4497480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1721,16 +1541,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>258120</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>72360</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>466200</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>412200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1745,8 +1565,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8441280" y="5037480"/>
-          <a:ext cx="2867400" cy="3286440"/>
+          <a:off x="10914840" y="4912200"/>
+          <a:ext cx="2867040" cy="3286080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1760,16 +1580,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>393840</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>178200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>167760</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>172800</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1777,8 +1597,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8577000" y="8469000"/>
-        <a:ext cx="6586200" cy="3718080"/>
+        <a:off x="11020680" y="8411760"/>
+        <a:ext cx="6585840" cy="3717720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1798,8 +1618,8 @@
   </sheetPr>
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A54" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10:J78"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A44" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10:K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1878,10 +1698,16 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
+      <c r="J7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1890,39 +1716,47 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
+      <c r="J8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="9" s="8">
       <c r="A9" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="0"/>
+        <v>20</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
       <c r="N9" s="0"/>
@@ -1938,60 +1772,63 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="10">
       <c r="A10" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>672</v>
       </c>
-      <c r="E11" s="10" t="n">
+      <c r="E11" s="11" t="n">
         <f aca="false">0.5*(F11+G11)</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="11" t="n">
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G11" s="11" t="n">
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
@@ -2001,33 +1838,41 @@
       <c r="I11" s="0" t="n">
         <v>73.9</v>
       </c>
-      <c r="J11" s="11" t="n">
+      <c r="J11" s="12" t="n">
         <f aca="false">(I11-H11)*SQRT(D11)/1.96</f>
         <v>67.4526072691432</v>
       </c>
+      <c r="K11" s="12" t="n">
+        <f aca="false">(I11-H11)*SQRT(D11)/TINV(1-0.95, D11-1)</f>
+        <v>67.3321758249646</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D11-1)</f>
+        <v>1.96350568844238</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>131</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="11" t="n">
         <f aca="false">0.5*(F12+G12)</f>
         <v>0.0438356164383562</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="11" t="n">
         <f aca="false">2/365</f>
         <v>0.00547945205479452</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="11" t="n">
         <f aca="false">30/365</f>
         <v>0.0821917808219178</v>
       </c>
@@ -2037,33 +1882,41 @@
       <c r="I12" s="0" t="n">
         <v>155.2</v>
       </c>
-      <c r="J12" s="11" t="n">
+      <c r="J12" s="12" t="n">
         <f aca="false">(I12-H12)*SQRT(D12)/1.96</f>
         <v>88.1772446163877</v>
       </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">(I12-H12)*SQRT(D12)/TINV(1-0.95, D12-1)</f>
+        <v>87.3580222348941</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D12-1)</f>
+        <v>1.97838040544702</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="E13" s="10" t="n">
+      <c r="E13" s="11" t="n">
         <f aca="false">0.5*(F13+G13)</f>
         <v>0.124657534246575</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="11" t="n">
         <f aca="false">31/365</f>
         <v>0.0849315068493151</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="11" t="n">
         <f aca="false">60/365</f>
         <v>0.164383561643836</v>
       </c>
@@ -2073,33 +1926,41 @@
       <c r="I13" s="0" t="n">
         <v>175.6</v>
       </c>
-      <c r="J13" s="11" t="n">
+      <c r="J13" s="12" t="n">
         <f aca="false">(I13-H13)*SQRT(D13)/1.96</f>
         <v>142.202582058215</v>
       </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">(I13-H13)*SQRT(D13)/TINV(1-0.95, D13-1)</f>
+        <v>140.550573104038</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D13-1)</f>
+        <v>1.98303752648373</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="11" t="n">
         <f aca="false">0.5*(F14+G14)</f>
         <v>0.206849315068493</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="11" t="n">
         <f aca="false">61/365</f>
         <v>0.167123287671233</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="11" t="n">
         <f aca="false">90/365</f>
         <v>0.246575342465753</v>
       </c>
@@ -2109,33 +1970,41 @@
       <c r="I14" s="0" t="n">
         <v>201.5</v>
       </c>
-      <c r="J14" s="11" t="n">
+      <c r="J14" s="12" t="n">
         <f aca="false">(I14-H14)*SQRT(D14)/1.96</f>
         <v>64.4569714319619</v>
       </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">(I14-H14)*SQRT(D14)/TINV(1-0.95, D14-1)</f>
+        <v>63.3278800762848</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D14-1)</f>
+        <v>1.99494541510724</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>74</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="11" t="n">
         <f aca="false">0.5*(F15+G15)</f>
         <v>0.289041095890411</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="11" t="n">
         <f aca="false">91/365</f>
         <v>0.249315068493151</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="11" t="n">
         <f aca="false">120/365</f>
         <v>0.328767123287671</v>
       </c>
@@ -2145,33 +2014,41 @@
       <c r="I15" s="0" t="n">
         <v>193.3</v>
       </c>
-      <c r="J15" s="11" t="n">
+      <c r="J15" s="12" t="n">
         <f aca="false">(I15-H15)*SQRT(D15)/1.96</f>
         <v>75.4897931597619</v>
       </c>
+      <c r="K15" s="12" t="n">
+        <f aca="false">(I15-H15)*SQRT(D15)/TINV(1-0.95, D15-1)</f>
+        <v>74.239943786708</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D15-1)</f>
+        <v>1.99299712588985</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>49</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="E16" s="11" t="n">
         <f aca="false">0.5*(F16+G16)</f>
         <v>0.371232876712329</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="11" t="n">
         <f aca="false">121/365</f>
         <v>0.331506849315068</v>
       </c>
-      <c r="G16" s="10" t="n">
+      <c r="G16" s="11" t="n">
         <f aca="false">150/365</f>
         <v>0.410958904109589</v>
       </c>
@@ -2181,33 +2058,41 @@
       <c r="I16" s="0" t="n">
         <v>249.4</v>
       </c>
-      <c r="J16" s="11" t="n">
+      <c r="J16" s="12" t="n">
         <f aca="false">(I16-H16)*SQRT(D16)/1.96</f>
         <v>121.071428571429</v>
       </c>
+      <c r="K16" s="12" t="n">
+        <f aca="false">(I16-H16)*SQRT(D16)/TINV(1-0.95, D16-1)</f>
+        <v>118.022430031198</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D16-1)</f>
+        <v>2.01063475762423</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="11" t="n">
         <f aca="false">0.5*(F17+G17)</f>
         <v>0.453424657534247</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="11" t="n">
         <f aca="false">151/365</f>
         <v>0.413698630136986</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="G17" s="11" t="n">
         <f aca="false">180/365</f>
         <v>0.493150684931507</v>
       </c>
@@ -2217,20 +2102,28 @@
       <c r="I17" s="0" t="n">
         <v>325.4</v>
       </c>
-      <c r="J17" s="11" t="n">
+      <c r="J17" s="12" t="n">
         <f aca="false">(I17-H17)*SQRT(D17)/1.96</f>
         <v>186.155970061409</v>
       </c>
+      <c r="K17" s="12" t="n">
+        <f aca="false">(I17-H17)*SQRT(D17)/TINV(1-0.95, D17-1)</f>
+        <v>180.667640152217</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D17-1)</f>
+        <v>2.01954097044138</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>46</v>
@@ -2251,20 +2144,28 @@
       <c r="I18" s="0" t="n">
         <v>329.6</v>
       </c>
-      <c r="J18" s="11" t="n">
+      <c r="J18" s="12" t="n">
         <f aca="false">(I18-H18)*SQRT(D18)/1.96</f>
         <v>126.649631317543</v>
       </c>
+      <c r="K18" s="12" t="n">
+        <f aca="false">(I18-H18)*SQRT(D18)/TINV(1-0.95, D18-1)</f>
+        <v>123.247534735701</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D18-1)</f>
+        <v>2.01410338888085</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>54</v>
@@ -2285,20 +2186,28 @@
       <c r="I19" s="0" t="n">
         <v>566.8</v>
       </c>
-      <c r="J19" s="11" t="n">
+      <c r="J19" s="12" t="n">
         <f aca="false">(I19-H19)*SQRT(D19)/1.96</f>
         <v>235.825874726115</v>
       </c>
+      <c r="K19" s="12" t="n">
+        <f aca="false">(I19-H19)*SQRT(D19)/TINV(1-0.95, D19-1)</f>
+        <v>230.447282727808</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D19-1)</f>
+        <v>2.00574599531787</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="4" t="n">
         <v>52</v>
@@ -2319,21 +2228,29 @@
       <c r="I20" s="0" t="n">
         <v>659.3</v>
       </c>
-      <c r="J20" s="11" t="n">
+      <c r="J20" s="12" t="n">
         <f aca="false">(I20-H20)*SQRT(D20)/1.96</f>
         <v>221.483864064216</v>
       </c>
+      <c r="K20" s="12" t="n">
+        <f aca="false">(I20-H20)*SQRT(D20)/TINV(1-0.95, D20-1)</f>
+        <v>216.234251334662</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D20-1)</f>
+        <v>2.00758377031584</v>
+      </c>
       <c r="U20" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>28</v>
@@ -2354,20 +2271,28 @@
       <c r="I21" s="0" t="n">
         <v>640.1</v>
       </c>
-      <c r="J21" s="11" t="n">
+      <c r="J21" s="12" t="n">
         <f aca="false">(I21-H21)*SQRT(D21)/1.96</f>
         <v>140.116829636992</v>
       </c>
+      <c r="K21" s="12" t="n">
+        <f aca="false">(I21-H21)*SQRT(D21)/TINV(1-0.95, D21-1)</f>
+        <v>133.845843446955</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D21-1)</f>
+        <v>2.05183051648029</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>44</v>
@@ -2388,20 +2313,28 @@
       <c r="I22" s="0" t="n">
         <v>699.9</v>
       </c>
-      <c r="J22" s="11" t="n">
+      <c r="J22" s="12" t="n">
         <f aca="false">(I22-H22)*SQRT(D22)/1.96</f>
         <v>162.108497406146</v>
       </c>
+      <c r="K22" s="12" t="n">
+        <f aca="false">(I22-H22)*SQRT(D22)/TINV(1-0.95, D22-1)</f>
+        <v>157.551387880463</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D22-1)</f>
+        <v>2.01669219922783</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>37</v>
@@ -2422,20 +2355,28 @@
       <c r="I23" s="0" t="n">
         <v>784.1</v>
       </c>
-      <c r="J23" s="11" t="n">
+      <c r="J23" s="12" t="n">
         <f aca="false">(I23-H23)*SQRT(D23)/1.96</f>
         <v>230.586355102632</v>
       </c>
+      <c r="K23" s="12" t="n">
+        <f aca="false">(I23-H23)*SQRT(D23)/TINV(1-0.95, D23-1)</f>
+        <v>222.844333538125</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D23-1)</f>
+        <v>2.02809400098045</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>34</v>
@@ -2456,20 +2397,28 @@
       <c r="I24" s="0" t="n">
         <v>832.9</v>
       </c>
-      <c r="J24" s="11" t="n">
+      <c r="J24" s="12" t="n">
         <f aca="false">(I24-H24)*SQRT(D24)/1.96</f>
         <v>238.890529161264</v>
       </c>
+      <c r="K24" s="12" t="n">
+        <f aca="false">(I24-H24)*SQRT(D24)/TINV(1-0.95, D24-1)</f>
+        <v>230.14102560108</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D24-1)</f>
+        <v>2.03451529744934</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D25" s="4" t="n">
         <v>30</v>
@@ -2490,20 +2439,28 @@
       <c r="I25" s="0" t="n">
         <v>968.9</v>
       </c>
-      <c r="J25" s="11" t="n">
+      <c r="J25" s="12" t="n">
         <f aca="false">(I25-H25)*SQRT(D25)/1.96</f>
         <v>340.370446449639</v>
       </c>
+      <c r="K25" s="12" t="n">
+        <f aca="false">(I25-H25)*SQRT(D25)/TINV(1-0.95, D25-1)</f>
+        <v>326.186390661555</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D25-1)</f>
+        <v>2.04522964213271</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>31</v>
@@ -2524,20 +2481,28 @@
       <c r="I26" s="0" t="n">
         <v>918.7</v>
       </c>
-      <c r="J26" s="11" t="n">
+      <c r="J26" s="12" t="n">
         <f aca="false">(I26-H26)*SQRT(D26)/1.96</f>
         <v>180.100132960931</v>
       </c>
+      <c r="K26" s="12" t="n">
+        <f aca="false">(I26-H26)*SQRT(D26)/TINV(1-0.95, D26-1)</f>
+        <v>172.844842280611</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D26-1)</f>
+        <v>2.04227245630124</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>28</v>
@@ -2558,20 +2523,28 @@
       <c r="I27" s="0" t="n">
         <v>1052.5</v>
       </c>
-      <c r="J27" s="11" t="n">
+      <c r="J27" s="12" t="n">
         <f aca="false">(I27-H27)*SQRT(D27)/1.96</f>
         <v>258.095740140587</v>
       </c>
+      <c r="K27" s="12" t="n">
+        <f aca="false">(I27-H27)*SQRT(D27)/TINV(1-0.95, D27-1)</f>
+        <v>246.544559412888</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D27-1)</f>
+        <v>2.05183051648029</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>17</v>
@@ -2592,20 +2565,28 @@
       <c r="I28" s="0" t="n">
         <v>1237.2</v>
       </c>
-      <c r="J28" s="11" t="n">
+      <c r="J28" s="12" t="n">
         <f aca="false">(I28-H28)*SQRT(D28)/1.96</f>
         <v>372.341681497105</v>
       </c>
+      <c r="K28" s="12" t="n">
+        <f aca="false">(I28-H28)*SQRT(D28)/TINV(1-0.95, D28-1)</f>
+        <v>344.255800484301</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D28-1)</f>
+        <v>2.11990529922126</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>24</v>
@@ -2626,20 +2607,28 @@
       <c r="I29" s="0" t="n">
         <v>1248.7</v>
       </c>
-      <c r="J29" s="11" t="n">
+      <c r="J29" s="12" t="n">
         <f aca="false">(I29-H29)*SQRT(D29)/1.96</f>
         <v>433.659663645797</v>
       </c>
+      <c r="K29" s="12" t="n">
+        <f aca="false">(I29-H29)*SQRT(D29)/TINV(1-0.95, D29-1)</f>
+        <v>410.881402734202</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D29-1)</f>
+        <v>2.06865761041905</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>21</v>
@@ -2660,20 +2649,28 @@
       <c r="I30" s="0" t="n">
         <v>1340</v>
       </c>
-      <c r="J30" s="11" t="n">
+      <c r="J30" s="12" t="n">
         <f aca="false">(I30-H30)*SQRT(D30)/1.96</f>
         <v>324.053567000448</v>
       </c>
+      <c r="K30" s="12" t="n">
+        <f aca="false">(I30-H30)*SQRT(D30)/TINV(1-0.95, D30-1)</f>
+        <v>304.485197069672</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D30-1)</f>
+        <v>2.08596344726587</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>28</v>
@@ -2694,20 +2691,28 @@
       <c r="I31" s="0" t="n">
         <v>1313.2</v>
       </c>
-      <c r="J31" s="11" t="n">
+      <c r="J31" s="12" t="n">
         <f aca="false">(I31-H31)*SQRT(D31)/1.96</f>
         <v>294.272339700041</v>
       </c>
+      <c r="K31" s="12" t="n">
+        <f aca="false">(I31-H31)*SQRT(D31)/TINV(1-0.95, D31-1)</f>
+        <v>281.10206041846</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D31-1)</f>
+        <v>2.05183051648029</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>30</v>
@@ -2728,20 +2733,28 @@
       <c r="I32" s="0" t="n">
         <v>1474.5</v>
       </c>
-      <c r="J32" s="11" t="n">
+      <c r="J32" s="12" t="n">
         <f aca="false">(I32-H32)*SQRT(D32)/1.96</f>
         <v>318.293873978768</v>
       </c>
+      <c r="K32" s="12" t="n">
+        <f aca="false">(I32-H32)*SQRT(D32)/TINV(1-0.95, D32-1)</f>
+        <v>305.02980210469</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D32-1)</f>
+        <v>2.04522964213271</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>40</v>
@@ -2762,20 +2775,28 @@
       <c r="I33" s="0" t="n">
         <v>1787.4</v>
       </c>
-      <c r="J33" s="11" t="n">
+      <c r="J33" s="12" t="n">
         <f aca="false">(I33-H33)*SQRT(D33)/1.96</f>
         <v>453.367358422099</v>
       </c>
+      <c r="K33" s="12" t="n">
+        <f aca="false">(I33-H33)*SQRT(D33)/TINV(1-0.95, D33-1)</f>
+        <v>439.31577173005</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D33-1)</f>
+        <v>2.02269092003676</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>56</v>
@@ -2796,20 +2817,28 @@
       <c r="I34" s="0" t="n">
         <v>1692.2</v>
       </c>
-      <c r="J34" s="11" t="n">
+      <c r="J34" s="12" t="n">
         <f aca="false">(I34-H34)*SQRT(D34)/1.96</f>
         <v>394.019430933746</v>
       </c>
+      <c r="K34" s="12" t="n">
+        <f aca="false">(I34-H34)*SQRT(D34)/TINV(1-0.95, D34-1)</f>
+        <v>385.359694089589</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D34-1)</f>
+        <v>2.00404478328915</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>56</v>
@@ -2830,20 +2859,28 @@
       <c r="I35" s="0" t="n">
         <v>1801.6</v>
       </c>
-      <c r="J35" s="11" t="n">
+      <c r="J35" s="12" t="n">
         <f aca="false">(I35-H35)*SQRT(D35)/1.96</f>
         <v>366.147901420021</v>
       </c>
+      <c r="K35" s="12" t="n">
+        <f aca="false">(I35-H35)*SQRT(D35)/TINV(1-0.95, D35-1)</f>
+        <v>358.100723480538</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D35-1)</f>
+        <v>2.00404478328915</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>69</v>
@@ -2864,20 +2901,28 @@
       <c r="I36" s="0" t="n">
         <v>1782.8</v>
       </c>
-      <c r="J36" s="11" t="n">
+      <c r="J36" s="12" t="n">
         <f aca="false">(I36-H36)*SQRT(D36)/1.96</f>
         <v>465.764266599334</v>
       </c>
+      <c r="K36" s="12" t="n">
+        <f aca="false">(I36-H36)*SQRT(D36)/TINV(1-0.95, D36-1)</f>
+        <v>457.485430194377</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D36-1)</f>
+        <v>1.99546893142984</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>486</v>
@@ -2898,20 +2943,28 @@
       <c r="I37" s="0" t="n">
         <v>1758.5</v>
       </c>
-      <c r="J37" s="11" t="n">
+      <c r="J37" s="12" t="n">
         <f aca="false">(I37-H37)*SQRT(D37)/1.96</f>
         <v>379.04604029905</v>
       </c>
+      <c r="K37" s="12" t="n">
+        <f aca="false">(I37-H37)*SQRT(D37)/TINV(1-0.95, D37-1)</f>
+        <v>378.107083313139</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D37-1)</f>
+        <v>1.96486728700309</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>463</v>
@@ -2932,20 +2985,28 @@
       <c r="I38" s="0" t="n">
         <v>1804.5</v>
       </c>
-      <c r="J38" s="11" t="n">
+      <c r="J38" s="12" t="n">
         <f aca="false">(I38-H38)*SQRT(D38)/1.96</f>
         <v>397.413846656567</v>
       </c>
+      <c r="K38" s="12" t="n">
+        <f aca="false">(I38-H38)*SQRT(D38)/TINV(1-0.95, D38-1)</f>
+        <v>396.380018745444</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D38-1)</f>
+        <v>1.96511202030873</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>657</v>
@@ -2966,20 +3027,28 @@
       <c r="I39" s="0" t="n">
         <v>1763.3</v>
       </c>
-      <c r="J39" s="11" t="n">
+      <c r="J39" s="12" t="n">
         <f aca="false">(I39-H39)*SQRT(D39)/1.96</f>
         <v>376.633634487466</v>
       </c>
+      <c r="K39" s="12" t="n">
+        <f aca="false">(I39-H39)*SQRT(D39)/TINV(1-0.95, D39-1)</f>
+        <v>375.945650198333</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D39-1)</f>
+        <v>1.96358681954689</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>856</v>
@@ -3000,20 +3069,28 @@
       <c r="I40" s="0" t="n">
         <v>1697.8</v>
       </c>
-      <c r="J40" s="11" t="n">
+      <c r="J40" s="12" t="n">
         <f aca="false">(I40-H40)*SQRT(D40)/1.96</f>
         <v>376.16757012843</v>
       </c>
+      <c r="K40" s="12" t="n">
+        <f aca="false">(I40-H40)*SQRT(D40)/TINV(1-0.95, D40-1)</f>
+        <v>375.641971138477</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D40-1)</f>
+        <v>1.96274243588166</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>939</v>
@@ -3034,20 +3111,28 @@
       <c r="I41" s="0" t="n">
         <v>1586.5</v>
       </c>
-      <c r="J41" s="11" t="n">
+      <c r="J41" s="12" t="n">
         <f aca="false">(I41-H41)*SQRT(D41)/1.96</f>
         <v>329.882426236264</v>
       </c>
+      <c r="K41" s="12" t="n">
+        <f aca="false">(I41-H41)*SQRT(D41)/TINV(1-0.95, D41-1)</f>
+        <v>329.462820136291</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D41-1)</f>
+        <v>1.9624962693988</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>580</v>
@@ -3068,20 +3153,28 @@
       <c r="I42" s="0" t="n">
         <v>1439.7</v>
       </c>
-      <c r="J42" s="11" t="n">
+      <c r="J42" s="12" t="n">
         <f aca="false">(I42-H42)*SQRT(D42)/1.96</f>
         <v>312.098471736046</v>
       </c>
+      <c r="K42" s="12" t="n">
+        <f aca="false">(I42-H42)*SQRT(D42)/TINV(1-0.95, D42-1)</f>
+        <v>311.451795480828</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D42-1)</f>
+        <v>1.96406960395997</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>168</v>
@@ -3102,20 +3195,28 @@
       <c r="I43" s="0" t="n">
         <v>1418</v>
       </c>
-      <c r="J43" s="11" t="n">
+      <c r="J43" s="12" t="n">
         <f aca="false">(I43-H43)*SQRT(D43)/1.96</f>
         <v>345.859937272174</v>
       </c>
+      <c r="K43" s="12" t="n">
+        <f aca="false">(I43-H43)*SQRT(D43)/TINV(1-0.95, D43-1)</f>
+        <v>343.359899329071</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D43-1)</f>
+        <v>1.97427095702805</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>14</v>
@@ -3136,33 +3237,41 @@
       <c r="I44" s="0" t="n">
         <v>1307.4</v>
       </c>
-      <c r="J44" s="11" t="n">
+      <c r="J44" s="12" t="n">
         <f aca="false">(I44-H44)*SQRT(D44)/1.96</f>
         <v>285.587727072134</v>
       </c>
+      <c r="K44" s="12" t="n">
+        <f aca="false">(I44-H44)*SQRT(D44)/TINV(1-0.95, D44-1)</f>
+        <v>259.100197268124</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D44-1)</f>
+        <v>2.16036865646279</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>563</v>
       </c>
-      <c r="E45" s="10" t="n">
+      <c r="E45" s="11" t="n">
         <f aca="false">0.5*(F45+G45)</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="F45" s="10" t="n">
+      <c r="F45" s="11" t="n">
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="G45" s="10" t="n">
+      <c r="G45" s="11" t="n">
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
@@ -3172,33 +3281,41 @@
       <c r="I45" s="0" t="n">
         <v>69.5</v>
       </c>
-      <c r="J45" s="11" t="n">
-        <f aca="false">(I45-H45)/1.96</f>
-        <v>1.93877551020408</v>
+      <c r="J45" s="12" t="n">
+        <f aca="false">(I45-H45)*SQRT(D45)/1.96</f>
+        <v>46.0025305788548</v>
+      </c>
+      <c r="K45" s="12" t="n">
+        <f aca="false">(I45-H45)*SQRT(D45)/TINV(1-0.95, D45-1)</f>
+        <v>45.9043033675443</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D45-1)</f>
+        <v>1.96419405850966</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>67</v>
       </c>
-      <c r="E46" s="10" t="n">
+      <c r="E46" s="11" t="n">
         <f aca="false">0.5*(F46+G46)</f>
         <v>0.0438356164383562</v>
       </c>
-      <c r="F46" s="10" t="n">
+      <c r="F46" s="11" t="n">
         <f aca="false">2/365</f>
         <v>0.00547945205479452</v>
       </c>
-      <c r="G46" s="10" t="n">
+      <c r="G46" s="11" t="n">
         <f aca="false">30/365</f>
         <v>0.0821917808219178</v>
       </c>
@@ -3208,33 +3325,41 @@
       <c r="I46" s="0" t="n">
         <v>132.6</v>
       </c>
-      <c r="J46" s="11" t="n">
-        <f aca="false">(I46-H46)/1.96</f>
-        <v>7.14285714285714</v>
+      <c r="J46" s="12" t="n">
+        <f aca="false">(I46-H46)*SQRT(D46)/1.96</f>
+        <v>58.4668055133746</v>
+      </c>
+      <c r="K46" s="12" t="n">
+        <f aca="false">(I46-H46)*SQRT(D46)/TINV(1-0.95, D46-1)</f>
+        <v>57.396063817639</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D46-1)</f>
+        <v>1.99656441895231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="E47" s="10" t="n">
+      <c r="E47" s="11" t="n">
         <f aca="false">0.5*(F47+G47)</f>
         <v>0.124657534246575</v>
       </c>
-      <c r="F47" s="10" t="n">
+      <c r="F47" s="11" t="n">
         <f aca="false">31/365</f>
         <v>0.0849315068493151</v>
       </c>
-      <c r="G47" s="10" t="n">
+      <c r="G47" s="11" t="n">
         <f aca="false">60/365</f>
         <v>0.164383561643836</v>
       </c>
@@ -3244,33 +3369,41 @@
       <c r="I47" s="0" t="n">
         <v>151.2</v>
       </c>
-      <c r="J47" s="11" t="n">
-        <f aca="false">(I47-H47)/1.96</f>
-        <v>6.22448979591836</v>
+      <c r="J47" s="12" t="n">
+        <f aca="false">(I47-H47)*SQRT(D47)/1.96</f>
+        <v>46.1620518074322</v>
+      </c>
+      <c r="K47" s="12" t="n">
+        <f aca="false">(I47-H47)*SQRT(D47)/TINV(1-0.95, D47-1)</f>
+        <v>45.1287127736941</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D47-1)</f>
+        <v>2.00487928818805</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D48" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E48" s="10" t="n">
+      <c r="E48" s="11" t="n">
         <f aca="false">0.5*(F48+G48)</f>
         <v>0.206849315068493</v>
       </c>
-      <c r="F48" s="10" t="n">
+      <c r="F48" s="11" t="n">
         <f aca="false">61/365</f>
         <v>0.167123287671233</v>
       </c>
-      <c r="G48" s="10" t="n">
+      <c r="G48" s="11" t="n">
         <f aca="false">90/365</f>
         <v>0.246575342465753</v>
       </c>
@@ -3280,33 +3413,41 @@
       <c r="I48" s="0" t="n">
         <v>174.9</v>
       </c>
-      <c r="J48" s="11" t="n">
-        <f aca="false">(I48-H48)/1.96</f>
-        <v>9.84693877551021</v>
+      <c r="J48" s="12" t="n">
+        <f aca="false">(I48-H48)*SQRT(D48)/1.96</f>
+        <v>68.221593032815</v>
+      </c>
+      <c r="K48" s="12" t="n">
+        <f aca="false">(I48-H48)*SQRT(D48)/TINV(1-0.95, D48-1)</f>
+        <v>66.4669829094464</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D48-1)</f>
+        <v>2.01174051372977</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D49" s="4" t="n">
         <v>44</v>
       </c>
-      <c r="E49" s="10" t="n">
+      <c r="E49" s="11" t="n">
         <f aca="false">0.5*(F49+G49)</f>
         <v>0.289041095890411</v>
       </c>
-      <c r="F49" s="10" t="n">
+      <c r="F49" s="11" t="n">
         <f aca="false">91/365</f>
         <v>0.249315068493151</v>
       </c>
-      <c r="G49" s="10" t="n">
+      <c r="G49" s="11" t="n">
         <f aca="false">120/365</f>
         <v>0.328767123287671</v>
       </c>
@@ -3316,33 +3457,41 @@
       <c r="I49" s="0" t="n">
         <v>221.4</v>
       </c>
-      <c r="J49" s="11" t="n">
-        <f aca="false">(I49-H49)/1.96</f>
-        <v>19.4387755102041</v>
+      <c r="J49" s="12" t="n">
+        <f aca="false">(I49-H49)*SQRT(D49)/1.96</f>
+        <v>128.942249502593</v>
+      </c>
+      <c r="K49" s="12" t="n">
+        <f aca="false">(I49-H49)*SQRT(D49)/TINV(1-0.95, D49-1)</f>
+        <v>125.317492238949</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D49-1)</f>
+        <v>2.01669219922783</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D50" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="E50" s="10" t="n">
+      <c r="E50" s="11" t="n">
         <f aca="false">0.5*(F50+G50)</f>
         <v>0.371232876712329</v>
       </c>
-      <c r="F50" s="10" t="n">
+      <c r="F50" s="11" t="n">
         <f aca="false">121/365</f>
         <v>0.331506849315068</v>
       </c>
-      <c r="G50" s="10" t="n">
+      <c r="G50" s="11" t="n">
         <f aca="false">150/365</f>
         <v>0.410958904109589</v>
       </c>
@@ -3352,33 +3501,41 @@
       <c r="I50" s="0" t="n">
         <v>232.2</v>
       </c>
-      <c r="J50" s="11" t="n">
-        <f aca="false">(I50-H50)/1.96</f>
-        <v>16.1734693877551</v>
+      <c r="J50" s="12" t="n">
+        <f aca="false">(I50-H50)*SQRT(D50)/1.96</f>
+        <v>97.0408163265306</v>
+      </c>
+      <c r="K50" s="12" t="n">
+        <f aca="false">(I50-H50)*SQRT(D50)/TINV(1-0.95, D50-1)</f>
+        <v>93.6896001208786</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D50-1)</f>
+        <v>2.03010792825034</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D51" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="E51" s="10" t="n">
+      <c r="E51" s="11" t="n">
         <f aca="false">0.5*(F51+G51)</f>
         <v>0.453424657534247</v>
       </c>
-      <c r="F51" s="10" t="n">
+      <c r="F51" s="11" t="n">
         <f aca="false">151/365</f>
         <v>0.413698630136986</v>
       </c>
-      <c r="G51" s="10" t="n">
+      <c r="G51" s="11" t="n">
         <f aca="false">180/365</f>
         <v>0.493150684931507</v>
       </c>
@@ -3388,20 +3545,28 @@
       <c r="I51" s="0" t="n">
         <v>252.5</v>
       </c>
-      <c r="J51" s="11" t="n">
-        <f aca="false">(I51-H51)/1.96</f>
-        <v>16.5816326530612</v>
+      <c r="J51" s="12" t="n">
+        <f aca="false">(I51-H51)*SQRT(D51)/1.96</f>
+        <v>96.6867023379961</v>
+      </c>
+      <c r="K51" s="12" t="n">
+        <f aca="false">(I51-H51)*SQRT(D51)/TINV(1-0.95, D51-1)</f>
+        <v>93.1454960402878</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D51-1)</f>
+        <v>2.03451529744934</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>42</v>
@@ -3422,20 +3587,28 @@
       <c r="I52" s="0" t="n">
         <v>313.5</v>
       </c>
-      <c r="J52" s="11" t="n">
-        <f aca="false">(I52-H52)/1.96</f>
-        <v>15.5612244897959</v>
+      <c r="J52" s="12" t="n">
+        <f aca="false">(I52-H52)*SQRT(D52)/1.96</f>
+        <v>100.848260868082</v>
+      </c>
+      <c r="K52" s="12" t="n">
+        <f aca="false">(I52-H52)*SQRT(D52)/TINV(1-0.95, D52-1)</f>
+        <v>97.8750093186968</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D52-1)</f>
+        <v>2.01954097044138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D53" s="4" t="n">
         <v>28</v>
@@ -3456,20 +3629,28 @@
       <c r="I53" s="0" t="n">
         <v>523.7</v>
       </c>
-      <c r="J53" s="11" t="n">
-        <f aca="false">(I53-H53)/1.96</f>
-        <v>56.1224489795919</v>
+      <c r="J53" s="12" t="n">
+        <f aca="false">(I53-H53)*SQRT(D53)/1.96</f>
+        <v>296.972085935822</v>
+      </c>
+      <c r="K53" s="12" t="n">
+        <f aca="false">(I53-H53)*SQRT(D53)/TINV(1-0.95, D53-1)</f>
+        <v>283.68097840395</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D53-1)</f>
+        <v>2.05183051648029</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>39</v>
@@ -3490,20 +3671,28 @@
       <c r="I54" s="0" t="n">
         <v>561.2</v>
       </c>
-      <c r="J54" s="11" t="n">
-        <f aca="false">(I54-H54)/1.96</f>
-        <v>28.5204081632653</v>
+      <c r="J54" s="12" t="n">
+        <f aca="false">(I54-H54)*SQRT(D54)/1.96</f>
+        <v>178.109891893097</v>
+      </c>
+      <c r="K54" s="12" t="n">
+        <f aca="false">(I54-H54)*SQRT(D54)/TINV(1-0.95, D54-1)</f>
+        <v>172.444375869901</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D54-1)</f>
+        <v>2.02439416391197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>31</v>
@@ -3524,20 +3713,28 @@
       <c r="I55" s="0" t="n">
         <v>580.5</v>
       </c>
-      <c r="J55" s="11" t="n">
-        <f aca="false">(I55-H55)/1.96</f>
-        <v>27.0918367346939</v>
+      <c r="J55" s="12" t="n">
+        <f aca="false">(I55-H55)*SQRT(D55)/1.96</f>
+        <v>150.840963095038</v>
+      </c>
+      <c r="K55" s="12" t="n">
+        <f aca="false">(I55-H55)*SQRT(D55)/TINV(1-0.95, D55-1)</f>
+        <v>144.764371058367</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D55-1)</f>
+        <v>2.04227245630124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>19</v>
@@ -3558,20 +3755,28 @@
       <c r="I56" s="0" t="n">
         <v>631.7</v>
       </c>
-      <c r="J56" s="11" t="n">
-        <f aca="false">(I56-H56)/1.96</f>
-        <v>39.9489795918368</v>
+      <c r="J56" s="12" t="n">
+        <f aca="false">(I56-H56)*SQRT(D56)/1.96</f>
+        <v>174.133564938385</v>
+      </c>
+      <c r="K56" s="12" t="n">
+        <f aca="false">(I56-H56)*SQRT(D56)/TINV(1-0.95, D56-1)</f>
+        <v>162.453332747215</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D56-1)</f>
+        <v>2.10092204024104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D57" s="4" t="n">
         <v>39</v>
@@ -3592,20 +3797,28 @@
       <c r="I57" s="0" t="n">
         <v>680.4</v>
       </c>
-      <c r="J57" s="11" t="n">
-        <f aca="false">(I57-H57)/1.96</f>
-        <v>31.4795918367347</v>
+      <c r="J57" s="12" t="n">
+        <f aca="false">(I57-H57)*SQRT(D57)/1.96</f>
+        <v>196.589988010807</v>
+      </c>
+      <c r="K57" s="12" t="n">
+        <f aca="false">(I57-H57)*SQRT(D57)/TINV(1-0.95, D57-1)</f>
+        <v>190.336636693612</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D57-1)</f>
+        <v>2.02439416391197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>20</v>
@@ -3626,20 +3839,28 @@
       <c r="I58" s="0" t="n">
         <v>689.4</v>
       </c>
-      <c r="J58" s="11" t="n">
-        <f aca="false">(I58-H58)/1.96</f>
-        <v>39.4897959183673</v>
+      <c r="J58" s="12" t="n">
+        <f aca="false">(I58-H58)*SQRT(D58)/1.96</f>
+        <v>176.603736182126</v>
+      </c>
+      <c r="K58" s="12" t="n">
+        <f aca="false">(I58-H58)*SQRT(D58)/TINV(1-0.95, D58-1)</f>
+        <v>165.379524515221</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D58-1)</f>
+        <v>2.09302405440831</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>26</v>
@@ -3660,20 +3881,28 @@
       <c r="I59" s="0" t="n">
         <v>833.9</v>
       </c>
-      <c r="J59" s="11" t="n">
-        <f aca="false">(I59-H59)/1.96</f>
-        <v>41.6326530612245</v>
+      <c r="J59" s="12" t="n">
+        <f aca="false">(I59-H59)*SQRT(D59)/1.96</f>
+        <v>212.285710361822</v>
+      </c>
+      <c r="K59" s="12" t="n">
+        <f aca="false">(I59-H59)*SQRT(D59)/TINV(1-0.95, D59-1)</f>
+        <v>202.025833288206</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D59-1)</f>
+        <v>2.0595385527533</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D60" s="4" t="n">
         <v>22</v>
@@ -3694,20 +3923,28 @@
       <c r="I60" s="0" t="n">
         <v>1026.8</v>
       </c>
-      <c r="J60" s="11" t="n">
-        <f aca="false">(I60-H60)/1.96</f>
-        <v>58.6734693877551</v>
+      <c r="J60" s="12" t="n">
+        <f aca="false">(I60-H60)*SQRT(D60)/1.96</f>
+        <v>275.202965499844</v>
+      </c>
+      <c r="K60" s="12" t="n">
+        <f aca="false">(I60-H60)*SQRT(D60)/TINV(1-0.95, D60-1)</f>
+        <v>259.374024532101</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D60-1)</f>
+        <v>2.07961384472768</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D61" s="4" t="n">
         <v>15</v>
@@ -3728,20 +3965,28 @@
       <c r="I61" s="0" t="n">
         <v>967.1</v>
       </c>
-      <c r="J61" s="11" t="n">
-        <f aca="false">(I61-H61)/1.96</f>
-        <v>61.9897959183674</v>
+      <c r="J61" s="12" t="n">
+        <f aca="false">(I61-H61)*SQRT(D61)/1.96</f>
+        <v>240.085447226633</v>
+      </c>
+      <c r="K61" s="12" t="n">
+        <f aca="false">(I61-H61)*SQRT(D61)/TINV(1-0.95, D61-1)</f>
+        <v>219.40059550679</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D61-1)</f>
+        <v>2.1447866879178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>10</v>
@@ -3762,20 +4007,28 @@
       <c r="I62" s="0" t="n">
         <v>1190.6</v>
       </c>
-      <c r="J62" s="11" t="n">
-        <f aca="false">(I62-H62)/1.96</f>
-        <v>48.7755102040816</v>
+      <c r="J62" s="12" t="n">
+        <f aca="false">(I62-H62)*SQRT(D62)/1.96</f>
+        <v>154.241706281682</v>
+      </c>
+      <c r="K62" s="12" t="n">
+        <f aca="false">(I62-H62)*SQRT(D62)/TINV(1-0.95, D62-1)</f>
+        <v>133.63958494296</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D62-1)</f>
+        <v>2.26215716279821</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>12</v>
@@ -3796,20 +4049,28 @@
       <c r="I63" s="0" t="n">
         <v>1181.7</v>
       </c>
-      <c r="J63" s="11" t="n">
-        <f aca="false">(I63-H63)/1.96</f>
-        <v>98.265306122449</v>
+      <c r="J63" s="12" t="n">
+        <f aca="false">(I63-H63)*SQRT(D63)/1.96</f>
+        <v>340.401005650781</v>
+      </c>
+      <c r="K63" s="12" t="n">
+        <f aca="false">(I63-H63)*SQRT(D63)/TINV(1-0.95, D63-1)</f>
+        <v>303.130608589725</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D63-1)</f>
+        <v>2.20098516009164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D64" s="4" t="n">
         <v>19</v>
@@ -3830,20 +4091,28 @@
       <c r="I64" s="0" t="n">
         <v>1187.1</v>
       </c>
-      <c r="J64" s="11" t="n">
-        <f aca="false">(I64-H64)/1.96</f>
-        <v>69.8469387755101</v>
+      <c r="J64" s="12" t="n">
+        <f aca="false">(I64-H64)*SQRT(D64)/1.96</f>
+        <v>304.455747638121</v>
+      </c>
+      <c r="K64" s="12" t="n">
+        <f aca="false">(I64-H64)*SQRT(D64)/TINV(1-0.95, D64-1)</f>
+        <v>284.033987906688</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D64-1)</f>
+        <v>2.10092204024104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>11</v>
@@ -3864,20 +4133,28 @@
       <c r="I65" s="0" t="n">
         <v>1307.5</v>
       </c>
-      <c r="J65" s="11" t="n">
-        <f aca="false">(I65-H65)/1.96</f>
-        <v>57.6530612244898</v>
+      <c r="J65" s="12" t="n">
+        <f aca="false">(I65-H65)*SQRT(D65)/1.96</f>
+        <v>191.213572097021</v>
+      </c>
+      <c r="K65" s="12" t="n">
+        <f aca="false">(I65-H65)*SQRT(D65)/TINV(1-0.95, D65-1)</f>
+        <v>168.202534135637</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D65-1)</f>
+        <v>2.22813885198628</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>28</v>
@@ -3898,20 +4175,28 @@
       <c r="I66" s="0" t="n">
         <v>1418.2</v>
       </c>
-      <c r="J66" s="11" t="n">
-        <f aca="false">(I66-H66)/1.96</f>
-        <v>56.4285714285715</v>
+      <c r="J66" s="12" t="n">
+        <f aca="false">(I66-H66)*SQRT(D66)/1.96</f>
+        <v>298.59193367729</v>
+      </c>
+      <c r="K66" s="12" t="n">
+        <f aca="false">(I66-H66)*SQRT(D66)/TINV(1-0.95, D66-1)</f>
+        <v>285.228329195245</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D66-1)</f>
+        <v>2.05183051648029</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>16</v>
@@ -3932,20 +4217,28 @@
       <c r="I67" s="0" t="n">
         <v>1560.6</v>
       </c>
-      <c r="J67" s="11" t="n">
-        <f aca="false">(I67-H67)/1.96</f>
-        <v>108.724489795918</v>
+      <c r="J67" s="12" t="n">
+        <f aca="false">(I67-H67)*SQRT(D67)/1.96</f>
+        <v>434.897959183673</v>
+      </c>
+      <c r="K67" s="12" t="n">
+        <f aca="false">(I67-H67)*SQRT(D67)/TINV(1-0.95, D67-1)</f>
+        <v>399.915635711722</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D67-1)</f>
+        <v>2.13144954555978</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>36</v>
@@ -3966,20 +4259,28 @@
       <c r="I68" s="0" t="n">
         <v>1546.3</v>
       </c>
-      <c r="J68" s="11" t="n">
-        <f aca="false">(I68-H68)/1.96</f>
-        <v>75.4591836734693</v>
+      <c r="J68" s="12" t="n">
+        <f aca="false">(I68-H68)*SQRT(D68)/1.96</f>
+        <v>452.755102040816</v>
+      </c>
+      <c r="K68" s="12" t="n">
+        <f aca="false">(I68-H68)*SQRT(D68)/TINV(1-0.95, D68-1)</f>
+        <v>437.119616967758</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D68-1)</f>
+        <v>2.03010792825034</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>26</v>
@@ -4000,20 +4301,28 @@
       <c r="I69" s="0" t="n">
         <v>1658.2</v>
       </c>
-      <c r="J69" s="11" t="n">
-        <f aca="false">(I69-H69)/1.96</f>
-        <v>78.469387755102</v>
+      <c r="J69" s="12" t="n">
+        <f aca="false">(I69-H69)*SQRT(D69)/1.96</f>
+        <v>400.116939382944</v>
+      </c>
+      <c r="K69" s="12" t="n">
+        <f aca="false">(I69-H69)*SQRT(D69)/TINV(1-0.95, D69-1)</f>
+        <v>380.779082839781</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D69-1)</f>
+        <v>2.0595385527533</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>36</v>
@@ -4034,20 +4343,28 @@
       <c r="I70" s="0" t="n">
         <v>1562.4</v>
       </c>
-      <c r="J70" s="11" t="n">
-        <f aca="false">(I70-H70)/1.96</f>
-        <v>54.1326530612246</v>
+      <c r="J70" s="12" t="n">
+        <f aca="false">(I70-H70)*SQRT(D70)/1.96</f>
+        <v>324.795918367347</v>
+      </c>
+      <c r="K70" s="12" t="n">
+        <f aca="false">(I70-H70)*SQRT(D70)/TINV(1-0.95, D70-1)</f>
+        <v>313.57938715537</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D70-1)</f>
+        <v>2.03010792825034</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>250</v>
@@ -4068,20 +4385,28 @@
       <c r="I71" s="0" t="n">
         <v>1587.7</v>
       </c>
-      <c r="J71" s="11" t="n">
+      <c r="J71" s="12" t="n">
         <f aca="false">(I71-H71)*SQRT(D71)/1.96</f>
         <v>358.176347223154</v>
       </c>
+      <c r="K71" s="12" t="n">
+        <f aca="false">(I71-H71)*SQRT(D71)/TINV(1-0.95, D71-1)</f>
+        <v>356.441990039241</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D71-1)</f>
+        <v>1.96953686764036</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>329</v>
@@ -4102,20 +4427,28 @@
       <c r="I72" s="0" t="n">
         <v>1631.3</v>
       </c>
-      <c r="J72" s="11" t="n">
+      <c r="J72" s="12" t="n">
         <f aca="false">(I72-H72)*SQRT(D72)/1.96</f>
         <v>367.394274869652</v>
       </c>
+      <c r="K72" s="12" t="n">
+        <f aca="false">(I72-H72)*SQRT(D72)/TINV(1-0.95, D72-1)</f>
+        <v>366.045355406977</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D72-1)</f>
+        <v>1.96722282664645</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>363</v>
@@ -4136,20 +4469,28 @@
       <c r="I73" s="0" t="n">
         <v>1594.9</v>
       </c>
-      <c r="J73" s="11" t="n">
+      <c r="J73" s="12" t="n">
         <f aca="false">(I73-H73)*SQRT(D73)/1.96</f>
         <v>359.665652388027</v>
       </c>
+      <c r="K73" s="12" t="n">
+        <f aca="false">(I73-H73)*SQRT(D73)/TINV(1-0.95, D73-1)</f>
+        <v>358.469751116069</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D73-1)</f>
+        <v>1.96653881250995</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>411</v>
@@ -4170,20 +4511,28 @@
       <c r="I74" s="0" t="n">
         <v>1530.5</v>
       </c>
-      <c r="J74" s="11" t="n">
+      <c r="J74" s="12" t="n">
         <f aca="false">(I74-H74)*SQRT(D74)/1.96</f>
         <v>365.123297512642</v>
       </c>
+      <c r="K74" s="12" t="n">
+        <f aca="false">(I74-H74)*SQRT(D74)/TINV(1-0.95, D74-1)</f>
+        <v>364.052159536486</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D74-1)</f>
+        <v>1.96576683966369</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>407</v>
@@ -4204,20 +4553,28 @@
       <c r="I75" s="0" t="n">
         <v>1442.1</v>
       </c>
-      <c r="J75" s="11" t="n">
+      <c r="J75" s="12" t="n">
         <f aca="false">(I75-H75)*SQRT(D75)/1.96</f>
         <v>345.844131459976</v>
       </c>
+      <c r="K75" s="12" t="n">
+        <f aca="false">(I75-H75)*SQRT(D75)/TINV(1-0.95, D75-1)</f>
+        <v>344.819493570784</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D75-1)</f>
+        <v>1.96582417844775</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>358</v>
@@ -4238,20 +4595,28 @@
       <c r="I76" s="0" t="n">
         <v>1281.7</v>
       </c>
-      <c r="J76" s="11" t="n">
+      <c r="J76" s="12" t="n">
         <f aca="false">(I76-H76)*SQRT(D76)/1.96</f>
         <v>283.813318926368</v>
       </c>
+      <c r="K76" s="12" t="n">
+        <f aca="false">(I76-H76)*SQRT(D76)/TINV(1-0.95, D76-1)</f>
+        <v>282.856340253732</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D76-1)</f>
+        <v>1.96663120436574</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>142</v>
@@ -4272,20 +4637,28 @@
       <c r="I77" s="0" t="n">
         <v>1216.8</v>
       </c>
-      <c r="J77" s="11" t="n">
+      <c r="J77" s="12" t="n">
         <f aca="false">(I77-H77)*SQRT(D77)/1.96</f>
         <v>268.118443975792</v>
       </c>
+      <c r="K77" s="12" t="n">
+        <f aca="false">(I77-H77)*SQRT(D77)/TINV(1-0.95, D77-1)</f>
+        <v>265.822135574155</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D77-1)</f>
+        <v>1.97693148863426</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>6</v>
@@ -4306,9 +4679,17 @@
       <c r="I78" s="0" t="n">
         <v>1302.2</v>
       </c>
-      <c r="J78" s="11" t="n">
+      <c r="J78" s="12" t="n">
         <f aca="false">(I78-H78)*SQRT(D78)/1.96</f>
         <v>333.930438403911</v>
+      </c>
+      <c r="K78" s="12" t="n">
+        <f aca="false">(I78-H78)*SQRT(D78)/TINV(1-0.95, D78-1)</f>
+        <v>254.613041373822</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <f aca="false">TINV(1-0.95, D78-1)</f>
+        <v>2.57058183563632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated preprocessing of population data for fits
</commit_message>
<xml_diff>
--- a/experimental_data/liver_volume/Kayser1987.xlsx
+++ b/experimental_data/liver_volume/Kayser1987.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="136" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="128" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Ducry1979" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
     <t>Size (n&gt;60)</t>
   </si>
   <si>
-    <t>size (t-distribution) </t>
+    <t>size (t-distribution)</t>
   </si>
   <si>
     <t>study</t>
@@ -415,7 +415,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -730,28 +730,28 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>44.5</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.5</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>64.5</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>74.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>84.5</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>94.5</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,7 +894,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1209,28 +1209,28 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>44.5</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.5</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>64.5</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>74.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>84.5</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>94.5</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,11 +1347,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="74802383"/>
-        <c:axId val="45850292"/>
+        <c:axId val="34806956"/>
+        <c:axId val="35728346"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74802383"/>
+        <c:axId val="34806956"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,11 +1385,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45850292"/>
+        <c:crossAx val="35728346"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45850292"/>
+        <c:axId val="35728346"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500"/>
@@ -1424,7 +1424,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74802383"/>
+        <c:crossAx val="34806956"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1464,15 +1464,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>255960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>508320</xdr:colOff>
+      <xdr:colOff>534960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1487,8 +1487,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10037520" y="634320"/>
-          <a:ext cx="4653360" cy="4182840"/>
+          <a:off x="10064520" y="625320"/>
+          <a:ext cx="4653000" cy="4182480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1503,15 +1503,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>508680</xdr:colOff>
+      <xdr:colOff>535680</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>763920</xdr:colOff>
+      <xdr:colOff>790560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1526,8 +1526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13065480" y="845640"/>
-          <a:ext cx="4319280" cy="4497480"/>
+          <a:off x="13092480" y="836640"/>
+          <a:ext cx="4318920" cy="4497120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1542,15 +1542,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>72360</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>412200</xdr:colOff>
+      <xdr:colOff>438840</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1565,8 +1565,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10914840" y="4912200"/>
-          <a:ext cx="2867040" cy="3286080"/>
+          <a:off x="10941840" y="4903200"/>
+          <a:ext cx="2866680" cy="3285720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1581,15 +1581,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>178200</xdr:colOff>
+      <xdr:colOff>205200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>172800</xdr:colOff>
+      <xdr:colOff>199440</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1597,8 +1597,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11020680" y="8411760"/>
-        <a:ext cx="6585840" cy="3717720"/>
+        <a:off x="11047680" y="8402760"/>
+        <a:ext cx="6585480" cy="3717360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1618,8 +1618,8 @@
   </sheetPr>
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A44" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10:K78"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A29" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G71" activeCellId="0" pane="topLeft" sqref="G71:G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1698,10 +1698,10 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1716,10 +1716,10 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1757,9 +1757,9 @@
       <c r="K9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="0"/>
-      <c r="M9" s="0"/>
-      <c r="N9" s="0"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1832,10 +1832,10 @@
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="4" t="n">
         <v>68.8</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="4" t="n">
         <v>73.9</v>
       </c>
       <c r="J11" s="12" t="n">
@@ -1846,7 +1846,7 @@
         <f aca="false">(I11-H11)*SQRT(D11)/TINV(1-0.95, D11-1)</f>
         <v>67.3321758249646</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="4" t="n">
         <f aca="false">TINV(1-0.95, D11-1)</f>
         <v>1.96350568844238</v>
       </c>
@@ -1876,10 +1876,10 @@
         <f aca="false">30/365</f>
         <v>0.0821917808219178</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="4" t="n">
         <v>140.1</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="4" t="n">
         <v>155.2</v>
       </c>
       <c r="J12" s="12" t="n">
@@ -1890,7 +1890,7 @@
         <f aca="false">(I12-H12)*SQRT(D12)/TINV(1-0.95, D12-1)</f>
         <v>87.3580222348941</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="4" t="n">
         <f aca="false">TINV(1-0.95, D12-1)</f>
         <v>1.97838040544702</v>
       </c>
@@ -1920,10 +1920,10 @@
         <f aca="false">60/365</f>
         <v>0.164383561643836</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="4" t="n">
         <v>148.4</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="4" t="n">
         <v>175.6</v>
       </c>
       <c r="J13" s="12" t="n">
@@ -1934,7 +1934,7 @@
         <f aca="false">(I13-H13)*SQRT(D13)/TINV(1-0.95, D13-1)</f>
         <v>140.550573104038</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="4" t="n">
         <f aca="false">TINV(1-0.95, D13-1)</f>
         <v>1.98303752648373</v>
       </c>
@@ -1964,10 +1964,10 @@
         <f aca="false">90/365</f>
         <v>0.246575342465753</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="4" t="n">
         <v>186.4</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="4" t="n">
         <v>201.5</v>
       </c>
       <c r="J14" s="12" t="n">
@@ -1978,7 +1978,7 @@
         <f aca="false">(I14-H14)*SQRT(D14)/TINV(1-0.95, D14-1)</f>
         <v>63.3278800762848</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="4" t="n">
         <f aca="false">TINV(1-0.95, D14-1)</f>
         <v>1.99494541510724</v>
       </c>
@@ -2008,10 +2008,10 @@
         <f aca="false">120/365</f>
         <v>0.328767123287671</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="4" t="n">
         <v>176.1</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="4" t="n">
         <v>193.3</v>
       </c>
       <c r="J15" s="12" t="n">
@@ -2022,7 +2022,7 @@
         <f aca="false">(I15-H15)*SQRT(D15)/TINV(1-0.95, D15-1)</f>
         <v>74.239943786708</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="4" t="n">
         <f aca="false">TINV(1-0.95, D15-1)</f>
         <v>1.99299712588985</v>
       </c>
@@ -2052,10 +2052,10 @@
         <f aca="false">150/365</f>
         <v>0.410958904109589</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="4" t="n">
         <v>215.5</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="4" t="n">
         <v>249.4</v>
       </c>
       <c r="J16" s="12" t="n">
@@ -2066,7 +2066,7 @@
         <f aca="false">(I16-H16)*SQRT(D16)/TINV(1-0.95, D16-1)</f>
         <v>118.022430031198</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="4" t="n">
         <f aca="false">TINV(1-0.95, D16-1)</f>
         <v>2.01063475762423</v>
       </c>
@@ -2096,10 +2096,10 @@
         <f aca="false">180/365</f>
         <v>0.493150684931507</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="4" t="n">
         <v>269.1</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="4" t="n">
         <v>325.4</v>
       </c>
       <c r="J17" s="12" t="n">
@@ -2110,7 +2110,7 @@
         <f aca="false">(I17-H17)*SQRT(D17)/TINV(1-0.95, D17-1)</f>
         <v>180.667640152217</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="4" t="n">
         <f aca="false">TINV(1-0.95, D17-1)</f>
         <v>2.01954097044138</v>
       </c>
@@ -2138,10 +2138,10 @@
       <c r="G18" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="4" t="n">
         <v>293</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="4" t="n">
         <v>329.6</v>
       </c>
       <c r="J18" s="12" t="n">
@@ -2152,7 +2152,7 @@
         <f aca="false">(I18-H18)*SQRT(D18)/TINV(1-0.95, D18-1)</f>
         <v>123.247534735701</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="4" t="n">
         <f aca="false">TINV(1-0.95, D18-1)</f>
         <v>2.01410338888085</v>
       </c>
@@ -2180,10 +2180,10 @@
       <c r="G19" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="4" t="n">
         <v>503.9</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="4" t="n">
         <v>566.8</v>
       </c>
       <c r="J19" s="12" t="n">
@@ -2194,7 +2194,7 @@
         <f aca="false">(I19-H19)*SQRT(D19)/TINV(1-0.95, D19-1)</f>
         <v>230.447282727808</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="4" t="n">
         <f aca="false">TINV(1-0.95, D19-1)</f>
         <v>2.00574599531787</v>
       </c>
@@ -2222,10 +2222,10 @@
       <c r="G20" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="4" t="n">
         <v>599.1</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="4" t="n">
         <v>659.3</v>
       </c>
       <c r="J20" s="12" t="n">
@@ -2236,7 +2236,7 @@
         <f aca="false">(I20-H20)*SQRT(D20)/TINV(1-0.95, D20-1)</f>
         <v>216.234251334662</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="4" t="n">
         <f aca="false">TINV(1-0.95, D20-1)</f>
         <v>2.00758377031584</v>
       </c>
@@ -2265,10 +2265,10 @@
       <c r="G21" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="4" t="n">
         <v>588.2</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="4" t="n">
         <v>640.1</v>
       </c>
       <c r="J21" s="12" t="n">
@@ -2279,7 +2279,7 @@
         <f aca="false">(I21-H21)*SQRT(D21)/TINV(1-0.95, D21-1)</f>
         <v>133.845843446955</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="4" t="n">
         <f aca="false">TINV(1-0.95, D21-1)</f>
         <v>2.05183051648029</v>
       </c>
@@ -2307,10 +2307,10 @@
       <c r="G22" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="4" t="n">
         <v>652</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="4" t="n">
         <v>699.9</v>
       </c>
       <c r="J22" s="12" t="n">
@@ -2321,7 +2321,7 @@
         <f aca="false">(I22-H22)*SQRT(D22)/TINV(1-0.95, D22-1)</f>
         <v>157.551387880463</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="4" t="n">
         <f aca="false">TINV(1-0.95, D22-1)</f>
         <v>2.01669219922783</v>
       </c>
@@ -2349,10 +2349,10 @@
       <c r="G23" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="4" t="n">
         <v>709.8</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="4" t="n">
         <v>784.1</v>
       </c>
       <c r="J23" s="12" t="n">
@@ -2363,7 +2363,7 @@
         <f aca="false">(I23-H23)*SQRT(D23)/TINV(1-0.95, D23-1)</f>
         <v>222.844333538125</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23" s="4" t="n">
         <f aca="false">TINV(1-0.95, D23-1)</f>
         <v>2.02809400098045</v>
       </c>
@@ -2391,10 +2391,10 @@
       <c r="G24" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="4" t="n">
         <v>752.6</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="4" t="n">
         <v>832.9</v>
       </c>
       <c r="J24" s="12" t="n">
@@ -2405,7 +2405,7 @@
         <f aca="false">(I24-H24)*SQRT(D24)/TINV(1-0.95, D24-1)</f>
         <v>230.14102560108</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24" s="4" t="n">
         <f aca="false">TINV(1-0.95, D24-1)</f>
         <v>2.03451529744934</v>
       </c>
@@ -2433,10 +2433,10 @@
       <c r="G25" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="4" t="n">
         <v>847.1</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="4" t="n">
         <v>968.9</v>
       </c>
       <c r="J25" s="12" t="n">
@@ -2447,7 +2447,7 @@
         <f aca="false">(I25-H25)*SQRT(D25)/TINV(1-0.95, D25-1)</f>
         <v>326.186390661555</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25" s="4" t="n">
         <f aca="false">TINV(1-0.95, D25-1)</f>
         <v>2.04522964213271</v>
       </c>
@@ -2475,10 +2475,10 @@
       <c r="G26" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="4" t="n">
         <v>855.3</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="4" t="n">
         <v>918.7</v>
       </c>
       <c r="J26" s="12" t="n">
@@ -2489,7 +2489,7 @@
         <f aca="false">(I26-H26)*SQRT(D26)/TINV(1-0.95, D26-1)</f>
         <v>172.844842280611</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="L26" s="4" t="n">
         <f aca="false">TINV(1-0.95, D26-1)</f>
         <v>2.04227245630124</v>
       </c>
@@ -2517,10 +2517,10 @@
       <c r="G27" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="4" t="n">
         <v>956.9</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="4" t="n">
         <v>1052.5</v>
       </c>
       <c r="J27" s="12" t="n">
@@ -2531,7 +2531,7 @@
         <f aca="false">(I27-H27)*SQRT(D27)/TINV(1-0.95, D27-1)</f>
         <v>246.544559412888</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27" s="4" t="n">
         <f aca="false">TINV(1-0.95, D27-1)</f>
         <v>2.05183051648029</v>
       </c>
@@ -2559,10 +2559,10 @@
       <c r="G28" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="4" t="n">
         <v>1060.2</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="4" t="n">
         <v>1237.2</v>
       </c>
       <c r="J28" s="12" t="n">
@@ -2573,7 +2573,7 @@
         <f aca="false">(I28-H28)*SQRT(D28)/TINV(1-0.95, D28-1)</f>
         <v>344.255800484301</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="L28" s="4" t="n">
         <f aca="false">TINV(1-0.95, D28-1)</f>
         <v>2.11990529922126</v>
       </c>
@@ -2601,10 +2601,10 @@
       <c r="G29" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="4" t="n">
         <v>1075.2</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="I29" s="4" t="n">
         <v>1248.7</v>
       </c>
       <c r="J29" s="12" t="n">
@@ -2615,7 +2615,7 @@
         <f aca="false">(I29-H29)*SQRT(D29)/TINV(1-0.95, D29-1)</f>
         <v>410.881402734202</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="L29" s="4" t="n">
         <f aca="false">TINV(1-0.95, D29-1)</f>
         <v>2.06865761041905</v>
       </c>
@@ -2643,10 +2643,10 @@
       <c r="G30" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="4" t="n">
         <v>1201.4</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="4" t="n">
         <v>1340</v>
       </c>
       <c r="J30" s="12" t="n">
@@ -2657,7 +2657,7 @@
         <f aca="false">(I30-H30)*SQRT(D30)/TINV(1-0.95, D30-1)</f>
         <v>304.485197069672</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30" s="4" t="n">
         <f aca="false">TINV(1-0.95, D30-1)</f>
         <v>2.08596344726587</v>
       </c>
@@ -2685,10 +2685,10 @@
       <c r="G31" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="4" t="n">
         <v>1204.2</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="I31" s="4" t="n">
         <v>1313.2</v>
       </c>
       <c r="J31" s="12" t="n">
@@ -2699,7 +2699,7 @@
         <f aca="false">(I31-H31)*SQRT(D31)/TINV(1-0.95, D31-1)</f>
         <v>281.10206041846</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31" s="4" t="n">
         <f aca="false">TINV(1-0.95, D31-1)</f>
         <v>2.05183051648029</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="C32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="4" t="n">
         <v>30</v>
       </c>
       <c r="E32" s="4" t="n">
@@ -2727,10 +2727,10 @@
       <c r="G32" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="4" t="n">
         <v>1360.6</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32" s="4" t="n">
         <v>1474.5</v>
       </c>
       <c r="J32" s="12" t="n">
@@ -2741,7 +2741,7 @@
         <f aca="false">(I32-H32)*SQRT(D32)/TINV(1-0.95, D32-1)</f>
         <v>305.02980210469</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="L32" s="4" t="n">
         <f aca="false">TINV(1-0.95, D32-1)</f>
         <v>2.04522964213271</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="C33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="4" t="n">
         <v>40</v>
       </c>
       <c r="E33" s="4" t="n">
@@ -2769,10 +2769,10 @@
       <c r="G33" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="4" t="n">
         <v>1646.9</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="I33" s="4" t="n">
         <v>1787.4</v>
       </c>
       <c r="J33" s="12" t="n">
@@ -2783,7 +2783,7 @@
         <f aca="false">(I33-H33)*SQRT(D33)/TINV(1-0.95, D33-1)</f>
         <v>439.31577173005</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33" s="4" t="n">
         <f aca="false">TINV(1-0.95, D33-1)</f>
         <v>2.02269092003676</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="C34" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="4" t="n">
         <v>56</v>
       </c>
       <c r="E34" s="4" t="n">
@@ -2811,10 +2811,10 @@
       <c r="G34" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="4" t="n">
         <v>1589</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I34" s="4" t="n">
         <v>1692.2</v>
       </c>
       <c r="J34" s="12" t="n">
@@ -2825,7 +2825,7 @@
         <f aca="false">(I34-H34)*SQRT(D34)/TINV(1-0.95, D34-1)</f>
         <v>385.359694089589</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L34" s="4" t="n">
         <f aca="false">TINV(1-0.95, D34-1)</f>
         <v>2.00404478328915</v>
       </c>
@@ -2840,7 +2840,7 @@
       <c r="C35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="4" t="n">
         <v>56</v>
       </c>
       <c r="E35" s="4" t="n">
@@ -2853,10 +2853,10 @@
       <c r="G35" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="4" t="n">
         <v>1705.7</v>
       </c>
-      <c r="I35" s="0" t="n">
+      <c r="I35" s="4" t="n">
         <v>1801.6</v>
       </c>
       <c r="J35" s="12" t="n">
@@ -2867,7 +2867,7 @@
         <f aca="false">(I35-H35)*SQRT(D35)/TINV(1-0.95, D35-1)</f>
         <v>358.100723480538</v>
       </c>
-      <c r="L35" s="0" t="n">
+      <c r="L35" s="4" t="n">
         <f aca="false">TINV(1-0.95, D35-1)</f>
         <v>2.00404478328915</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="C36" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="4" t="n">
         <v>69</v>
       </c>
       <c r="E36" s="4" t="n">
@@ -2895,10 +2895,10 @@
       <c r="G36" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="4" t="n">
         <v>1672.9</v>
       </c>
-      <c r="I36" s="0" t="n">
+      <c r="I36" s="4" t="n">
         <v>1782.8</v>
       </c>
       <c r="J36" s="12" t="n">
@@ -2909,7 +2909,7 @@
         <f aca="false">(I36-H36)*SQRT(D36)/TINV(1-0.95, D36-1)</f>
         <v>457.485430194377</v>
       </c>
-      <c r="L36" s="0" t="n">
+      <c r="L36" s="4" t="n">
         <f aca="false">TINV(1-0.95, D36-1)</f>
         <v>1.99546893142984</v>
       </c>
@@ -2924,23 +2924,23 @@
       <c r="C37" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="4" t="n">
         <v>486</v>
       </c>
       <c r="E37" s="4" t="n">
         <f aca="false">0.5*(F37+G37)</f>
-        <v>24.5</v>
-      </c>
-      <c r="F37" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F37" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="H37" s="0" t="n">
+      <c r="G37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H37" s="4" t="n">
         <v>1724.8</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="I37" s="4" t="n">
         <v>1758.5</v>
       </c>
       <c r="J37" s="12" t="n">
@@ -2951,7 +2951,7 @@
         <f aca="false">(I37-H37)*SQRT(D37)/TINV(1-0.95, D37-1)</f>
         <v>378.107083313139</v>
       </c>
-      <c r="L37" s="0" t="n">
+      <c r="L37" s="4" t="n">
         <f aca="false">TINV(1-0.95, D37-1)</f>
         <v>1.96486728700309</v>
       </c>
@@ -2966,23 +2966,23 @@
       <c r="C38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="4" t="n">
         <v>463</v>
       </c>
       <c r="E38" s="4" t="n">
         <f aca="false">0.5*(F38+G38)</f>
-        <v>34.5</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="H38" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H38" s="4" t="n">
         <v>1768.3</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="I38" s="4" t="n">
         <v>1804.5</v>
       </c>
       <c r="J38" s="12" t="n">
@@ -2993,7 +2993,7 @@
         <f aca="false">(I38-H38)*SQRT(D38)/TINV(1-0.95, D38-1)</f>
         <v>396.380018745444</v>
       </c>
-      <c r="L38" s="0" t="n">
+      <c r="L38" s="4" t="n">
         <f aca="false">TINV(1-0.95, D38-1)</f>
         <v>1.96511202030873</v>
       </c>
@@ -3008,23 +3008,23 @@
       <c r="C39" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="4" t="n">
         <v>657</v>
       </c>
       <c r="E39" s="4" t="n">
         <f aca="false">0.5*(F39+G39)</f>
-        <v>44.5</v>
-      </c>
-      <c r="F39" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F39" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="H39" s="0" t="n">
+      <c r="G39" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="n">
         <v>1734.5</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="I39" s="4" t="n">
         <v>1763.3</v>
       </c>
       <c r="J39" s="12" t="n">
@@ -3035,7 +3035,7 @@
         <f aca="false">(I39-H39)*SQRT(D39)/TINV(1-0.95, D39-1)</f>
         <v>375.945650198333</v>
       </c>
-      <c r="L39" s="0" t="n">
+      <c r="L39" s="4" t="n">
         <f aca="false">TINV(1-0.95, D39-1)</f>
         <v>1.96358681954689</v>
       </c>
@@ -3050,23 +3050,23 @@
       <c r="C40" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="4" t="n">
         <v>856</v>
       </c>
       <c r="E40" s="4" t="n">
         <f aca="false">0.5*(F40+G40)</f>
-        <v>54.5</v>
-      </c>
-      <c r="F40" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="F40" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H40" s="0" t="n">
+      <c r="G40" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="H40" s="4" t="n">
         <v>1672.6</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="I40" s="4" t="n">
         <v>1697.8</v>
       </c>
       <c r="J40" s="12" t="n">
@@ -3077,7 +3077,7 @@
         <f aca="false">(I40-H40)*SQRT(D40)/TINV(1-0.95, D40-1)</f>
         <v>375.641971138477</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="L40" s="4" t="n">
         <f aca="false">TINV(1-0.95, D40-1)</f>
         <v>1.96274243588166</v>
       </c>
@@ -3092,23 +3092,23 @@
       <c r="C41" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="4" t="n">
         <v>939</v>
       </c>
       <c r="E41" s="4" t="n">
         <f aca="false">0.5*(F41+G41)</f>
-        <v>64.5</v>
-      </c>
-      <c r="F41" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F41" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <v>69</v>
-      </c>
-      <c r="H41" s="0" t="n">
+      <c r="G41" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="H41" s="4" t="n">
         <v>1565.4</v>
       </c>
-      <c r="I41" s="0" t="n">
+      <c r="I41" s="4" t="n">
         <v>1586.5</v>
       </c>
       <c r="J41" s="12" t="n">
@@ -3119,7 +3119,7 @@
         <f aca="false">(I41-H41)*SQRT(D41)/TINV(1-0.95, D41-1)</f>
         <v>329.462820136291</v>
       </c>
-      <c r="L41" s="0" t="n">
+      <c r="L41" s="4" t="n">
         <f aca="false">TINV(1-0.95, D41-1)</f>
         <v>1.9624962693988</v>
       </c>
@@ -3134,23 +3134,23 @@
       <c r="C42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="4" t="n">
         <v>580</v>
       </c>
       <c r="E42" s="4" t="n">
         <f aca="false">0.5*(F42+G42)</f>
-        <v>74.5</v>
-      </c>
-      <c r="F42" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F42" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="H42" s="0" t="n">
+      <c r="G42" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="H42" s="4" t="n">
         <v>1414.3</v>
       </c>
-      <c r="I42" s="0" t="n">
+      <c r="I42" s="4" t="n">
         <v>1439.7</v>
       </c>
       <c r="J42" s="12" t="n">
@@ -3161,7 +3161,7 @@
         <f aca="false">(I42-H42)*SQRT(D42)/TINV(1-0.95, D42-1)</f>
         <v>311.451795480828</v>
       </c>
-      <c r="L42" s="0" t="n">
+      <c r="L42" s="4" t="n">
         <f aca="false">TINV(1-0.95, D42-1)</f>
         <v>1.96406960395997</v>
       </c>
@@ -3176,23 +3176,23 @@
       <c r="C43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="4" t="n">
         <v>168</v>
       </c>
       <c r="E43" s="4" t="n">
         <f aca="false">0.5*(F43+G43)</f>
-        <v>84.5</v>
-      </c>
-      <c r="F43" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="F43" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="H43" s="0" t="n">
+      <c r="G43" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="H43" s="4" t="n">
         <v>1365.7</v>
       </c>
-      <c r="I43" s="0" t="n">
+      <c r="I43" s="4" t="n">
         <v>1418</v>
       </c>
       <c r="J43" s="12" t="n">
@@ -3203,7 +3203,7 @@
         <f aca="false">(I43-H43)*SQRT(D43)/TINV(1-0.95, D43-1)</f>
         <v>343.359899329071</v>
       </c>
-      <c r="L43" s="0" t="n">
+      <c r="L43" s="4" t="n">
         <f aca="false">TINV(1-0.95, D43-1)</f>
         <v>1.97427095702805</v>
       </c>
@@ -3218,23 +3218,23 @@
       <c r="C44" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="4" t="n">
         <v>14</v>
       </c>
       <c r="E44" s="4" t="n">
         <f aca="false">0.5*(F44+G44)</f>
-        <v>94.5</v>
-      </c>
-      <c r="F44" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="F44" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="H44" s="0" t="n">
+      <c r="G44" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H44" s="4" t="n">
         <v>1157.8</v>
       </c>
-      <c r="I44" s="0" t="n">
+      <c r="I44" s="4" t="n">
         <v>1307.4</v>
       </c>
       <c r="J44" s="12" t="n">
@@ -3245,7 +3245,7 @@
         <f aca="false">(I44-H44)*SQRT(D44)/TINV(1-0.95, D44-1)</f>
         <v>259.100197268124</v>
       </c>
-      <c r="L44" s="0" t="n">
+      <c r="L44" s="4" t="n">
         <f aca="false">TINV(1-0.95, D44-1)</f>
         <v>2.16036865646279</v>
       </c>
@@ -3275,10 +3275,10 @@
         <f aca="false">1/365</f>
         <v>0.00273972602739726</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45" s="4" t="n">
         <v>65.7</v>
       </c>
-      <c r="I45" s="0" t="n">
+      <c r="I45" s="4" t="n">
         <v>69.5</v>
       </c>
       <c r="J45" s="12" t="n">
@@ -3289,7 +3289,7 @@
         <f aca="false">(I45-H45)*SQRT(D45)/TINV(1-0.95, D45-1)</f>
         <v>45.9043033675443</v>
       </c>
-      <c r="L45" s="0" t="n">
+      <c r="L45" s="4" t="n">
         <f aca="false">TINV(1-0.95, D45-1)</f>
         <v>1.96419405850966</v>
       </c>
@@ -3319,10 +3319,10 @@
         <f aca="false">30/365</f>
         <v>0.0821917808219178</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46" s="4" t="n">
         <v>118.6</v>
       </c>
-      <c r="I46" s="0" t="n">
+      <c r="I46" s="4" t="n">
         <v>132.6</v>
       </c>
       <c r="J46" s="12" t="n">
@@ -3333,7 +3333,7 @@
         <f aca="false">(I46-H46)*SQRT(D46)/TINV(1-0.95, D46-1)</f>
         <v>57.396063817639</v>
       </c>
-      <c r="L46" s="0" t="n">
+      <c r="L46" s="4" t="n">
         <f aca="false">TINV(1-0.95, D46-1)</f>
         <v>1.99656441895231</v>
       </c>
@@ -3363,10 +3363,10 @@
         <f aca="false">60/365</f>
         <v>0.164383561643836</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47" s="4" t="n">
         <v>139</v>
       </c>
-      <c r="I47" s="0" t="n">
+      <c r="I47" s="4" t="n">
         <v>151.2</v>
       </c>
       <c r="J47" s="12" t="n">
@@ -3377,7 +3377,7 @@
         <f aca="false">(I47-H47)*SQRT(D47)/TINV(1-0.95, D47-1)</f>
         <v>45.1287127736941</v>
       </c>
-      <c r="L47" s="0" t="n">
+      <c r="L47" s="4" t="n">
         <f aca="false">TINV(1-0.95, D47-1)</f>
         <v>2.00487928818805</v>
       </c>
@@ -3407,10 +3407,10 @@
         <f aca="false">90/365</f>
         <v>0.246575342465753</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48" s="4" t="n">
         <v>155.6</v>
       </c>
-      <c r="I48" s="0" t="n">
+      <c r="I48" s="4" t="n">
         <v>174.9</v>
       </c>
       <c r="J48" s="12" t="n">
@@ -3421,7 +3421,7 @@
         <f aca="false">(I48-H48)*SQRT(D48)/TINV(1-0.95, D48-1)</f>
         <v>66.4669829094464</v>
       </c>
-      <c r="L48" s="0" t="n">
+      <c r="L48" s="4" t="n">
         <f aca="false">TINV(1-0.95, D48-1)</f>
         <v>2.01174051372977</v>
       </c>
@@ -3451,10 +3451,10 @@
         <f aca="false">120/365</f>
         <v>0.328767123287671</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="H49" s="4" t="n">
         <v>183.3</v>
       </c>
-      <c r="I49" s="0" t="n">
+      <c r="I49" s="4" t="n">
         <v>221.4</v>
       </c>
       <c r="J49" s="12" t="n">
@@ -3465,7 +3465,7 @@
         <f aca="false">(I49-H49)*SQRT(D49)/TINV(1-0.95, D49-1)</f>
         <v>125.317492238949</v>
       </c>
-      <c r="L49" s="0" t="n">
+      <c r="L49" s="4" t="n">
         <f aca="false">TINV(1-0.95, D49-1)</f>
         <v>2.01669219922783</v>
       </c>
@@ -3495,10 +3495,10 @@
         <f aca="false">150/365</f>
         <v>0.410958904109589</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50" s="4" t="n">
         <v>200.5</v>
       </c>
-      <c r="I50" s="0" t="n">
+      <c r="I50" s="4" t="n">
         <v>232.2</v>
       </c>
       <c r="J50" s="12" t="n">
@@ -3509,7 +3509,7 @@
         <f aca="false">(I50-H50)*SQRT(D50)/TINV(1-0.95, D50-1)</f>
         <v>93.6896001208786</v>
       </c>
-      <c r="L50" s="0" t="n">
+      <c r="L50" s="4" t="n">
         <f aca="false">TINV(1-0.95, D50-1)</f>
         <v>2.03010792825034</v>
       </c>
@@ -3539,10 +3539,10 @@
         <f aca="false">180/365</f>
         <v>0.493150684931507</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51" s="4" t="n">
         <v>220</v>
       </c>
-      <c r="I51" s="0" t="n">
+      <c r="I51" s="4" t="n">
         <v>252.5</v>
       </c>
       <c r="J51" s="12" t="n">
@@ -3553,7 +3553,7 @@
         <f aca="false">(I51-H51)*SQRT(D51)/TINV(1-0.95, D51-1)</f>
         <v>93.1454960402878</v>
       </c>
-      <c r="L51" s="0" t="n">
+      <c r="L51" s="4" t="n">
         <f aca="false">TINV(1-0.95, D51-1)</f>
         <v>2.03451529744934</v>
       </c>
@@ -3581,10 +3581,10 @@
       <c r="G52" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52" s="4" t="n">
         <v>283</v>
       </c>
-      <c r="I52" s="0" t="n">
+      <c r="I52" s="4" t="n">
         <v>313.5</v>
       </c>
       <c r="J52" s="12" t="n">
@@ -3595,7 +3595,7 @@
         <f aca="false">(I52-H52)*SQRT(D52)/TINV(1-0.95, D52-1)</f>
         <v>97.8750093186968</v>
       </c>
-      <c r="L52" s="0" t="n">
+      <c r="L52" s="4" t="n">
         <f aca="false">TINV(1-0.95, D52-1)</f>
         <v>2.01954097044138</v>
       </c>
@@ -3623,10 +3623,10 @@
       <c r="G53" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="H53" s="4" t="n">
         <v>413.7</v>
       </c>
-      <c r="I53" s="0" t="n">
+      <c r="I53" s="4" t="n">
         <v>523.7</v>
       </c>
       <c r="J53" s="12" t="n">
@@ -3637,7 +3637,7 @@
         <f aca="false">(I53-H53)*SQRT(D53)/TINV(1-0.95, D53-1)</f>
         <v>283.68097840395</v>
       </c>
-      <c r="L53" s="0" t="n">
+      <c r="L53" s="4" t="n">
         <f aca="false">TINV(1-0.95, D53-1)</f>
         <v>2.05183051648029</v>
       </c>
@@ -3665,10 +3665,10 @@
       <c r="G54" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="H54" s="4" t="n">
         <v>505.3</v>
       </c>
-      <c r="I54" s="0" t="n">
+      <c r="I54" s="4" t="n">
         <v>561.2</v>
       </c>
       <c r="J54" s="12" t="n">
@@ -3679,7 +3679,7 @@
         <f aca="false">(I54-H54)*SQRT(D54)/TINV(1-0.95, D54-1)</f>
         <v>172.444375869901</v>
       </c>
-      <c r="L54" s="0" t="n">
+      <c r="L54" s="4" t="n">
         <f aca="false">TINV(1-0.95, D54-1)</f>
         <v>2.02439416391197</v>
       </c>
@@ -3707,10 +3707,10 @@
       <c r="G55" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="H55" s="4" t="n">
         <v>527.4</v>
       </c>
-      <c r="I55" s="0" t="n">
+      <c r="I55" s="4" t="n">
         <v>580.5</v>
       </c>
       <c r="J55" s="12" t="n">
@@ -3721,7 +3721,7 @@
         <f aca="false">(I55-H55)*SQRT(D55)/TINV(1-0.95, D55-1)</f>
         <v>144.764371058367</v>
       </c>
-      <c r="L55" s="0" t="n">
+      <c r="L55" s="4" t="n">
         <f aca="false">TINV(1-0.95, D55-1)</f>
         <v>2.04227245630124</v>
       </c>
@@ -3749,10 +3749,10 @@
       <c r="G56" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="H56" s="4" t="n">
         <v>553.4</v>
       </c>
-      <c r="I56" s="0" t="n">
+      <c r="I56" s="4" t="n">
         <v>631.7</v>
       </c>
       <c r="J56" s="12" t="n">
@@ -3763,7 +3763,7 @@
         <f aca="false">(I56-H56)*SQRT(D56)/TINV(1-0.95, D56-1)</f>
         <v>162.453332747215</v>
       </c>
-      <c r="L56" s="0" t="n">
+      <c r="L56" s="4" t="n">
         <f aca="false">TINV(1-0.95, D56-1)</f>
         <v>2.10092204024104</v>
       </c>
@@ -3791,10 +3791,10 @@
       <c r="G57" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="H57" s="4" t="n">
         <v>618.7</v>
       </c>
-      <c r="I57" s="0" t="n">
+      <c r="I57" s="4" t="n">
         <v>680.4</v>
       </c>
       <c r="J57" s="12" t="n">
@@ -3805,7 +3805,7 @@
         <f aca="false">(I57-H57)*SQRT(D57)/TINV(1-0.95, D57-1)</f>
         <v>190.336636693612</v>
       </c>
-      <c r="L57" s="0" t="n">
+      <c r="L57" s="4" t="n">
         <f aca="false">TINV(1-0.95, D57-1)</f>
         <v>2.02439416391197</v>
       </c>
@@ -3833,10 +3833,10 @@
       <c r="G58" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="H58" s="4" t="n">
         <v>612</v>
       </c>
-      <c r="I58" s="0" t="n">
+      <c r="I58" s="4" t="n">
         <v>689.4</v>
       </c>
       <c r="J58" s="12" t="n">
@@ -3847,7 +3847,7 @@
         <f aca="false">(I58-H58)*SQRT(D58)/TINV(1-0.95, D58-1)</f>
         <v>165.379524515221</v>
       </c>
-      <c r="L58" s="0" t="n">
+      <c r="L58" s="4" t="n">
         <f aca="false">TINV(1-0.95, D58-1)</f>
         <v>2.09302405440831</v>
       </c>
@@ -3875,10 +3875,10 @@
       <c r="G59" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="H59" s="4" t="n">
         <v>752.3</v>
       </c>
-      <c r="I59" s="0" t="n">
+      <c r="I59" s="4" t="n">
         <v>833.9</v>
       </c>
       <c r="J59" s="12" t="n">
@@ -3889,7 +3889,7 @@
         <f aca="false">(I59-H59)*SQRT(D59)/TINV(1-0.95, D59-1)</f>
         <v>202.025833288206</v>
       </c>
-      <c r="L59" s="0" t="n">
+      <c r="L59" s="4" t="n">
         <f aca="false">TINV(1-0.95, D59-1)</f>
         <v>2.0595385527533</v>
       </c>
@@ -3917,10 +3917,10 @@
       <c r="G60" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60" s="4" t="n">
         <v>911.8</v>
       </c>
-      <c r="I60" s="0" t="n">
+      <c r="I60" s="4" t="n">
         <v>1026.8</v>
       </c>
       <c r="J60" s="12" t="n">
@@ -3931,7 +3931,7 @@
         <f aca="false">(I60-H60)*SQRT(D60)/TINV(1-0.95, D60-1)</f>
         <v>259.374024532101</v>
       </c>
-      <c r="L60" s="0" t="n">
+      <c r="L60" s="4" t="n">
         <f aca="false">TINV(1-0.95, D60-1)</f>
         <v>2.07961384472768</v>
       </c>
@@ -3959,10 +3959,10 @@
       <c r="G61" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="H61" s="4" t="n">
         <v>845.6</v>
       </c>
-      <c r="I61" s="0" t="n">
+      <c r="I61" s="4" t="n">
         <v>967.1</v>
       </c>
       <c r="J61" s="12" t="n">
@@ -3973,7 +3973,7 @@
         <f aca="false">(I61-H61)*SQRT(D61)/TINV(1-0.95, D61-1)</f>
         <v>219.40059550679</v>
       </c>
-      <c r="L61" s="0" t="n">
+      <c r="L61" s="4" t="n">
         <f aca="false">TINV(1-0.95, D61-1)</f>
         <v>2.1447866879178</v>
       </c>
@@ -4001,10 +4001,10 @@
       <c r="G62" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="H62" s="4" t="n">
         <v>1095</v>
       </c>
-      <c r="I62" s="0" t="n">
+      <c r="I62" s="4" t="n">
         <v>1190.6</v>
       </c>
       <c r="J62" s="12" t="n">
@@ -4015,7 +4015,7 @@
         <f aca="false">(I62-H62)*SQRT(D62)/TINV(1-0.95, D62-1)</f>
         <v>133.63958494296</v>
       </c>
-      <c r="L62" s="0" t="n">
+      <c r="L62" s="4" t="n">
         <f aca="false">TINV(1-0.95, D62-1)</f>
         <v>2.26215716279821</v>
       </c>
@@ -4043,10 +4043,10 @@
       <c r="G63" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="H63" s="4" t="n">
         <v>989.1</v>
       </c>
-      <c r="I63" s="0" t="n">
+      <c r="I63" s="4" t="n">
         <v>1181.7</v>
       </c>
       <c r="J63" s="12" t="n">
@@ -4057,7 +4057,7 @@
         <f aca="false">(I63-H63)*SQRT(D63)/TINV(1-0.95, D63-1)</f>
         <v>303.130608589725</v>
       </c>
-      <c r="L63" s="0" t="n">
+      <c r="L63" s="4" t="n">
         <f aca="false">TINV(1-0.95, D63-1)</f>
         <v>2.20098516009164</v>
       </c>
@@ -4085,10 +4085,10 @@
       <c r="G64" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="H64" s="4" t="n">
         <v>1050.2</v>
       </c>
-      <c r="I64" s="0" t="n">
+      <c r="I64" s="4" t="n">
         <v>1187.1</v>
       </c>
       <c r="J64" s="12" t="n">
@@ -4099,7 +4099,7 @@
         <f aca="false">(I64-H64)*SQRT(D64)/TINV(1-0.95, D64-1)</f>
         <v>284.033987906688</v>
       </c>
-      <c r="L64" s="0" t="n">
+      <c r="L64" s="4" t="n">
         <f aca="false">TINV(1-0.95, D64-1)</f>
         <v>2.10092204024104</v>
       </c>
@@ -4127,10 +4127,10 @@
       <c r="G65" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="H65" s="4" t="n">
         <v>1194.5</v>
       </c>
-      <c r="I65" s="0" t="n">
+      <c r="I65" s="4" t="n">
         <v>1307.5</v>
       </c>
       <c r="J65" s="12" t="n">
@@ -4141,7 +4141,7 @@
         <f aca="false">(I65-H65)*SQRT(D65)/TINV(1-0.95, D65-1)</f>
         <v>168.202534135637</v>
       </c>
-      <c r="L65" s="0" t="n">
+      <c r="L65" s="4" t="n">
         <f aca="false">TINV(1-0.95, D65-1)</f>
         <v>2.22813885198628</v>
       </c>
@@ -4156,7 +4156,7 @@
       <c r="C66" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66" s="4" t="n">
         <v>28</v>
       </c>
       <c r="E66" s="4" t="n">
@@ -4169,10 +4169,10 @@
       <c r="G66" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="H66" s="4" t="n">
         <v>1307.6</v>
       </c>
-      <c r="I66" s="0" t="n">
+      <c r="I66" s="4" t="n">
         <v>1418.2</v>
       </c>
       <c r="J66" s="12" t="n">
@@ -4183,7 +4183,7 @@
         <f aca="false">(I66-H66)*SQRT(D66)/TINV(1-0.95, D66-1)</f>
         <v>285.228329195245</v>
       </c>
-      <c r="L66" s="0" t="n">
+      <c r="L66" s="4" t="n">
         <f aca="false">TINV(1-0.95, D66-1)</f>
         <v>2.05183051648029</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="C67" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="4" t="n">
         <v>16</v>
       </c>
       <c r="E67" s="4" t="n">
@@ -4211,10 +4211,10 @@
       <c r="G67" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="H67" s="4" t="n">
         <v>1347.5</v>
       </c>
-      <c r="I67" s="0" t="n">
+      <c r="I67" s="4" t="n">
         <v>1560.6</v>
       </c>
       <c r="J67" s="12" t="n">
@@ -4225,7 +4225,7 @@
         <f aca="false">(I67-H67)*SQRT(D67)/TINV(1-0.95, D67-1)</f>
         <v>399.915635711722</v>
       </c>
-      <c r="L67" s="0" t="n">
+      <c r="L67" s="4" t="n">
         <f aca="false">TINV(1-0.95, D67-1)</f>
         <v>2.13144954555978</v>
       </c>
@@ -4240,7 +4240,7 @@
       <c r="C68" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="4" t="n">
         <v>36</v>
       </c>
       <c r="E68" s="4" t="n">
@@ -4253,10 +4253,10 @@
       <c r="G68" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="H68" s="4" t="n">
         <v>1398.4</v>
       </c>
-      <c r="I68" s="0" t="n">
+      <c r="I68" s="4" t="n">
         <v>1546.3</v>
       </c>
       <c r="J68" s="12" t="n">
@@ -4267,7 +4267,7 @@
         <f aca="false">(I68-H68)*SQRT(D68)/TINV(1-0.95, D68-1)</f>
         <v>437.119616967758</v>
       </c>
-      <c r="L68" s="0" t="n">
+      <c r="L68" s="4" t="n">
         <f aca="false">TINV(1-0.95, D68-1)</f>
         <v>2.03010792825034</v>
       </c>
@@ -4282,7 +4282,7 @@
       <c r="C69" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="4" t="n">
         <v>26</v>
       </c>
       <c r="E69" s="4" t="n">
@@ -4295,10 +4295,10 @@
       <c r="G69" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="H69" s="4" t="n">
         <v>1504.4</v>
       </c>
-      <c r="I69" s="0" t="n">
+      <c r="I69" s="4" t="n">
         <v>1658.2</v>
       </c>
       <c r="J69" s="12" t="n">
@@ -4309,7 +4309,7 @@
         <f aca="false">(I69-H69)*SQRT(D69)/TINV(1-0.95, D69-1)</f>
         <v>380.779082839781</v>
       </c>
-      <c r="L69" s="0" t="n">
+      <c r="L69" s="4" t="n">
         <f aca="false">TINV(1-0.95, D69-1)</f>
         <v>2.0595385527533</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="C70" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="4" t="n">
         <v>36</v>
       </c>
       <c r="E70" s="4" t="n">
@@ -4337,10 +4337,10 @@
       <c r="G70" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="H70" s="4" t="n">
         <v>1456.3</v>
       </c>
-      <c r="I70" s="0" t="n">
+      <c r="I70" s="4" t="n">
         <v>1562.4</v>
       </c>
       <c r="J70" s="12" t="n">
@@ -4351,7 +4351,7 @@
         <f aca="false">(I70-H70)*SQRT(D70)/TINV(1-0.95, D70-1)</f>
         <v>313.57938715537</v>
       </c>
-      <c r="L70" s="0" t="n">
+      <c r="L70" s="4" t="n">
         <f aca="false">TINV(1-0.95, D70-1)</f>
         <v>2.03010792825034</v>
       </c>
@@ -4366,23 +4366,23 @@
       <c r="C71" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="4" t="n">
         <v>250</v>
       </c>
       <c r="E71" s="4" t="n">
         <f aca="false">0.5*(F71+G71)</f>
-        <v>24.5</v>
-      </c>
-      <c r="F71" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F71" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G71" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="H71" s="0" t="n">
+      <c r="G71" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H71" s="4" t="n">
         <v>1543.3</v>
       </c>
-      <c r="I71" s="0" t="n">
+      <c r="I71" s="4" t="n">
         <v>1587.7</v>
       </c>
       <c r="J71" s="12" t="n">
@@ -4393,7 +4393,7 @@
         <f aca="false">(I71-H71)*SQRT(D71)/TINV(1-0.95, D71-1)</f>
         <v>356.441990039241</v>
       </c>
-      <c r="L71" s="0" t="n">
+      <c r="L71" s="4" t="n">
         <f aca="false">TINV(1-0.95, D71-1)</f>
         <v>1.96953686764036</v>
       </c>
@@ -4408,23 +4408,23 @@
       <c r="C72" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="4" t="n">
         <v>329</v>
       </c>
       <c r="E72" s="4" t="n">
         <f aca="false">0.5*(F72+G72)</f>
-        <v>34.5</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="G72" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="H72" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F72" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G72" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H72" s="4" t="n">
         <v>1591.6</v>
       </c>
-      <c r="I72" s="0" t="n">
+      <c r="I72" s="4" t="n">
         <v>1631.3</v>
       </c>
       <c r="J72" s="12" t="n">
@@ -4435,7 +4435,7 @@
         <f aca="false">(I72-H72)*SQRT(D72)/TINV(1-0.95, D72-1)</f>
         <v>366.045355406977</v>
       </c>
-      <c r="L72" s="0" t="n">
+      <c r="L72" s="4" t="n">
         <f aca="false">TINV(1-0.95, D72-1)</f>
         <v>1.96722282664645</v>
       </c>
@@ -4450,23 +4450,23 @@
       <c r="C73" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D73" s="4" t="n">
         <v>363</v>
       </c>
       <c r="E73" s="4" t="n">
         <f aca="false">0.5*(F73+G73)</f>
-        <v>44.5</v>
-      </c>
-      <c r="F73" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F73" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="H73" s="0" t="n">
+      <c r="G73" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H73" s="4" t="n">
         <v>1557.9</v>
       </c>
-      <c r="I73" s="0" t="n">
+      <c r="I73" s="4" t="n">
         <v>1594.9</v>
       </c>
       <c r="J73" s="12" t="n">
@@ -4477,7 +4477,7 @@
         <f aca="false">(I73-H73)*SQRT(D73)/TINV(1-0.95, D73-1)</f>
         <v>358.469751116069</v>
       </c>
-      <c r="L73" s="0" t="n">
+      <c r="L73" s="4" t="n">
         <f aca="false">TINV(1-0.95, D73-1)</f>
         <v>1.96653881250995</v>
       </c>
@@ -4492,23 +4492,23 @@
       <c r="C74" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D74" s="0" t="n">
+      <c r="D74" s="4" t="n">
         <v>411</v>
       </c>
       <c r="E74" s="4" t="n">
         <f aca="false">0.5*(F74+G74)</f>
-        <v>54.5</v>
-      </c>
-      <c r="F74" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="F74" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G74" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="H74" s="0" t="n">
+      <c r="G74" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="H74" s="4" t="n">
         <v>1495.2</v>
       </c>
-      <c r="I74" s="0" t="n">
+      <c r="I74" s="4" t="n">
         <v>1530.5</v>
       </c>
       <c r="J74" s="12" t="n">
@@ -4519,7 +4519,7 @@
         <f aca="false">(I74-H74)*SQRT(D74)/TINV(1-0.95, D74-1)</f>
         <v>364.052159536486</v>
       </c>
-      <c r="L74" s="0" t="n">
+      <c r="L74" s="4" t="n">
         <f aca="false">TINV(1-0.95, D74-1)</f>
         <v>1.96576683966369</v>
       </c>
@@ -4534,23 +4534,23 @@
       <c r="C75" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="4" t="n">
         <v>407</v>
       </c>
       <c r="E75" s="4" t="n">
         <f aca="false">0.5*(F75+G75)</f>
-        <v>64.5</v>
-      </c>
-      <c r="F75" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F75" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="G75" s="0" t="n">
-        <v>69</v>
-      </c>
-      <c r="H75" s="0" t="n">
+      <c r="G75" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="H75" s="4" t="n">
         <v>1408.5</v>
       </c>
-      <c r="I75" s="0" t="n">
+      <c r="I75" s="4" t="n">
         <v>1442.1</v>
       </c>
       <c r="J75" s="12" t="n">
@@ -4561,7 +4561,7 @@
         <f aca="false">(I75-H75)*SQRT(D75)/TINV(1-0.95, D75-1)</f>
         <v>344.819493570784</v>
       </c>
-      <c r="L75" s="0" t="n">
+      <c r="L75" s="4" t="n">
         <f aca="false">TINV(1-0.95, D75-1)</f>
         <v>1.96582417844775</v>
       </c>
@@ -4576,23 +4576,23 @@
       <c r="C76" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="4" t="n">
         <v>358</v>
       </c>
       <c r="E76" s="4" t="n">
         <f aca="false">0.5*(F76+G76)</f>
-        <v>74.5</v>
-      </c>
-      <c r="F76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F76" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="G76" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="H76" s="0" t="n">
+      <c r="G76" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="H76" s="4" t="n">
         <v>1252.3</v>
       </c>
-      <c r="I76" s="0" t="n">
+      <c r="I76" s="4" t="n">
         <v>1281.7</v>
       </c>
       <c r="J76" s="12" t="n">
@@ -4603,7 +4603,7 @@
         <f aca="false">(I76-H76)*SQRT(D76)/TINV(1-0.95, D76-1)</f>
         <v>282.856340253732</v>
       </c>
-      <c r="L76" s="0" t="n">
+      <c r="L76" s="4" t="n">
         <f aca="false">TINV(1-0.95, D76-1)</f>
         <v>1.96663120436574</v>
       </c>
@@ -4618,23 +4618,23 @@
       <c r="C77" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="4" t="n">
         <v>142</v>
       </c>
       <c r="E77" s="4" t="n">
         <f aca="false">0.5*(F77+G77)</f>
-        <v>84.5</v>
-      </c>
-      <c r="F77" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="F77" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="G77" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="H77" s="0" t="n">
+      <c r="G77" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="H77" s="4" t="n">
         <v>1172.7</v>
       </c>
-      <c r="I77" s="0" t="n">
+      <c r="I77" s="4" t="n">
         <v>1216.8</v>
       </c>
       <c r="J77" s="12" t="n">
@@ -4645,7 +4645,7 @@
         <f aca="false">(I77-H77)*SQRT(D77)/TINV(1-0.95, D77-1)</f>
         <v>265.822135574155</v>
       </c>
-      <c r="L77" s="0" t="n">
+      <c r="L77" s="4" t="n">
         <f aca="false">TINV(1-0.95, D77-1)</f>
         <v>1.97693148863426</v>
       </c>
@@ -4660,23 +4660,23 @@
       <c r="C78" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="4" t="n">
         <v>6</v>
       </c>
       <c r="E78" s="4" t="n">
         <f aca="false">0.5*(F78+G78)</f>
-        <v>94.5</v>
-      </c>
-      <c r="F78" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="F78" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="H78" s="0" t="n">
+      <c r="G78" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H78" s="4" t="n">
         <v>1035</v>
       </c>
-      <c r="I78" s="0" t="n">
+      <c r="I78" s="4" t="n">
         <v>1302.2</v>
       </c>
       <c r="J78" s="12" t="n">
@@ -4687,7 +4687,7 @@
         <f aca="false">(I78-H78)*SQRT(D78)/TINV(1-0.95, D78-1)</f>
         <v>254.613041373822</v>
       </c>
-      <c r="L78" s="0" t="n">
+      <c r="L78" s="4" t="n">
         <f aca="false">TINV(1-0.95, D78-1)</f>
         <v>2.57058183563632</v>
       </c>

</xml_diff>